<commit_message>
Updates including more crops
</commit_message>
<xml_diff>
--- a/CWatM_settings/cwatm_settings.xlsx
+++ b/CWatM_settings/cwatm_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\FUSE\CWatM_settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C738CC-1DE1-414B-A1C0-2A9C6D8CD3EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B927AA-C6E2-481C-9121-B2FE72157E6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1032" yWindow="-96" windowWidth="22104" windowHeight="13152" tabRatio="633" xr2:uid="{3B47940C-5F20-42D1-80D0-733DA86DBAA8}"/>
+    <workbookView xWindow="996" yWindow="-96" windowWidth="22140" windowHeight="13152" tabRatio="633" xr2:uid="{3B47940C-5F20-42D1-80D0-733DA86DBAA8}"/>
   </bookViews>
   <sheets>
     <sheet name="CWatM_input" sheetId="13" r:id="rId1"/>
@@ -18,12 +18,13 @@
     <sheet name="CWatM_input_all" sheetId="12" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="7" r:id="rId4"/>
     <sheet name="Crops" sheetId="4" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="6" r:id="rId6"/>
-    <sheet name="Notepad" sheetId="1" r:id="rId7"/>
-    <sheet name="All_Settings_Template" sheetId="2" r:id="rId8"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId9"/>
-    <sheet name="Sheet4" sheetId="10" r:id="rId10"/>
-    <sheet name="Sheet5" sheetId="9" r:id="rId11"/>
+    <sheet name="Crops (2)" sheetId="14" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId7"/>
+    <sheet name="Notepad" sheetId="1" r:id="rId8"/>
+    <sheet name="All_Settings_Template" sheetId="2" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId10"/>
+    <sheet name="Sheet4" sheetId="10" r:id="rId11"/>
+    <sheet name="Sheet5" sheetId="9" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2411" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2467" uniqueCount="763">
   <si>
     <t>PathRoot</t>
   </si>
@@ -2163,12 +2164,6 @@
     <t xml:space="preserve"> 28/05/1992</t>
   </si>
   <si>
-    <t xml:space="preserve"> $(FILE_PATHS:PathMaps)/init/UB</t>
-  </si>
-  <si>
-    <t>fracVegCover[1], fracVegCover[3], frac_totalIrr, frac_totalnonIrr, fracCrops_Irr[0],  fracCrops_Irr[1], fracCrops_Irr[2], fracCrops_Irr[3], fracCrops_Irr[4], fracCrops_Irr[5], fracCrops_Irr[6], fracCrops_Irr[7],  fracCrops_nonIrr[0], fracCrops_nonIrr[1], fracCrops_nonIrr[2], fracCrops_nonIrr[3], fracCrops_nonIrr[4], fracCrops_nonIrr[5], fracCrops_nonIrr[6], fracCrops_nonIrr[7],  fracCrops_IrrLandDemand[0],  fracCrops_IrrLandDemand[1], fracCrops_IrrLandDemand[2], fracCrops_IrrLandDemand[3], fracCrops_IrrLandDemand[4], fracCrops_IrrLandDemand[5], fracCrops_IrrLandDemand[6], fracCrops_IrrLandDemand[7], fracCrops_nonIrrLandDemand[0],  fracCrops_nonIrrLandDemand[1], fracCrops_nonIrrLandDemand[2], fracCrops_nonIrrLandDemand[3], fracCrops_nonIrrLandDemand[4], fracCrops_nonIrrLandDemand[5], fracCrops_nonIrrLandDemand[6], fracCrops_nonIrrLandDemand[7]</t>
-  </si>
-  <si>
     <t xml:space="preserve"> C:/GitHub/FUSE/Input/landsurface/waterDemand/Agents_raster.tif</t>
   </si>
   <si>
@@ -2181,29 +2176,224 @@
     <t>ETRefAverage_segments</t>
   </si>
   <si>
-    <t xml:space="preserve"> 01/06/2004</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 31/12/2007</t>
   </si>
   <si>
+    <t>, lakeResInflowDis, lakeResOutflowDis, lakeResStorage, act_bigLakeResAbst_alloc, gwstorage_cell_avail, allowedPumping, gwstorage_cell_avail</t>
+  </si>
+  <si>
+    <t>availableGWStorageFraction</t>
+  </si>
+  <si>
+    <t>modflowtotalSoilThickness, cellArea, adminSegments_area, adminSegments, availableGWStorageFraction</t>
+  </si>
+  <si>
+    <t>C:/GitHub/FUSE/Input/landsurface/waterDemand/availableGWStorageFraction_totalend.nc</t>
+  </si>
+  <si>
+    <t>C:/GitHub/FUSE/Input/landcover/crops/Sugar_JY2.tif</t>
+  </si>
+  <si>
+    <t>$(FILE_PATHS:PathMaps)/landcover/crops/Sugar_JY2.tif</t>
+  </si>
+  <si>
+    <t>$(FILE_PATHS:PathMaps)/landcover/crops/Sorghum_1km.tif</t>
+  </si>
+  <si>
+    <t>$(FILE_PATHS:PathMaps)/landcover/crops/Groundnut_30sec.tif</t>
+  </si>
+  <si>
+    <t>$(FILE_PATHS:PathMaps)/landcover/crops/Wheat_30sec.tif</t>
+  </si>
+  <si>
+    <t>$(FILE_PATHS:PathMaps)/landcover/crops/Maize_30sec.tif</t>
+  </si>
+  <si>
+    <t>$(FILE_PATHS:PathMaps)/landsurface/waterDemand/availableGWStorageFraction_Anjuli.nc</t>
+  </si>
+  <si>
+    <t>75.12083 17.97083 Nira</t>
+  </si>
+  <si>
+    <t>$(FILE_PATHS:PathMaps)/init/Nira_20070427.nc</t>
+  </si>
+  <si>
+    <t>75.89583 17.3875 Bhima</t>
+  </si>
+  <si>
+    <t>Cotton</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/0378-3774(94)90025-6</t>
+  </si>
+  <si>
+    <t>Soybean</t>
+  </si>
+  <si>
+    <t>Gram</t>
+  </si>
+  <si>
+    <t>FruitVegK</t>
+  </si>
+  <si>
+    <t>FruitVegR</t>
+  </si>
+  <si>
+    <t>SpicesK</t>
+  </si>
+  <si>
+    <t>SpicesR</t>
+  </si>
+  <si>
+    <t>Tomato</t>
+  </si>
+  <si>
+    <t>$(FILE_PATHS:PathMaps)/landcover/crops/Gram.tif</t>
+  </si>
+  <si>
+    <t>$(FILE_PATHS:PathMaps)/landcover/crops/Soybean.tif</t>
+  </si>
+  <si>
+    <t>$(FILE_PATHS:PathMaps)/landcover/crops/Cotton.tif</t>
+  </si>
+  <si>
+    <t>$(FILE_PATHS:PathMaps)/landcover/crops/CondimentsSpicesRabi.tif</t>
+  </si>
+  <si>
+    <t>$(FILE_PATHS:PathMaps)/landcover/crops/CondimentsSpicesKharif.tif</t>
+  </si>
+  <si>
+    <t>$(FILE_PATHS:PathMaps)/landcover/crops/FruitVegRabi.tif</t>
+  </si>
+  <si>
+    <t>$(FILE_PATHS:PathMaps)/landcover/crops/FruitVegKharif.tif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modflowWaterLevel, areaCrops_Irr_segment[0], areaCrops_Irr_segment[1], areaCrops_Irr_segment[2], areaCrops_Irr_segment[3], areaCrops_Irr_segment[4], areaCrops_Irr_segment[5], areaCrops_Irr_segment[6], areaCrops_Irr_segment[7], areaCrops_Irr_segment[8], areaCrops_Irr_segment[9], areaCrops_Irr_segment[10], areaCrops_Irr_segment[11], areaCrops_Irr_segment[12], areaCrops_Irr_segment[13], areaCrops_Irr_segment[14], areaCrops_Irr_segment[15], head_development_segments, allowedPumping, gwstorage_cell_avail, fracVegCover[1], fracVegCover[3], frac_totalIrr, frac_totalnonIrr, fracCrops_Irr[0],  fracCrops_Irr[1], fracCrops_Irr[2], fracCrops_Irr[3], fracCrops_Irr[4], fracCrops_Irr[5], fracCrops_Irr[6], fracCrops_Irr[7], fracCrops_Irr[8], fracCrops_Irr[9], fracCrops_Irr[10], fracCrops_Irr[11], fracCrops_Irr[12], fracCrops_Irr[13], fracCrops_Irr[14], fracCrops_Irr[15], fracCrops_nonIrr[0], fracCrops_nonIrr[1], fracCrops_nonIrr[2], fracCrops_nonIrr[3], fracCrops_nonIrr[4], fracCrops_nonIrr[5], fracCrops_nonIrr[6], fracCrops_nonIrr[7],  fracCrops_nonIrr[8], fracCrops_nonIrr[9], fracCrops_nonIrr[10], fracCrops_nonIrr[11], fracCrops_nonIrr[12], fracCrops_nonIrr[13], fracCrops_nonIrr[14], fracCrops_nonIrr[15], fracCrops_IrrLandDemand[0],  fracCrops_IrrLandDemand[1], fracCrops_IrrLandDemand[2], fracCrops_IrrLandDemand[3], fracCrops_IrrLandDemand[4], fracCrops_IrrLandDemand[5], fracCrops_IrrLandDemand[6], fracCrops_IrrLandDemand[7],fracCrops_IrrLandDemand[8], fracCrops_IrrLandDemand[9], fracCrops_IrrLandDemand[10], fracCrops_IrrLandDemand[11], fracCrops_IrrLandDemand[12], fracCrops_IrrLandDemand[13], fracCrops_IrrLandDemand[14], fracCrops_IrrLandDemand[15], fracCrops_nonIrrLandDemand[0],  fracCrops_nonIrrLandDemand[1], fracCrops_nonIrrLandDemand[2], fracCrops_nonIrrLandDemand[3], fracCrops_nonIrrLandDemand[4], fracCrops_nonIrrLandDemand[5], fracCrops_nonIrrLandDemand[6], fracCrops_nonIrrLandDemand[7], fracCrops_nonIrrLandDemand[8], fracCrops_nonIrrLandDemand[9], fracCrops_nonIrrLandDemand[10], fracCrops_nonIrrLandDemand[11], fracCrops_nonIrrLandDemand[12], fracCrops_nonIrrLandDemand[13], fracCrops_nonIrrLandDemand[14], fracCrops_nonIrrLandDemand[15]     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 01/07/2006</t>
+  </si>
+  <si>
+    <t>FarmerAgent_rev_raster.tif</t>
+  </si>
+  <si>
+    <t>$(FILE_PATHS:PathMaps)/landsurface/waterDemand/AgentsRaster_10July20.tif</t>
+  </si>
+  <si>
+    <t>Chili</t>
+  </si>
+  <si>
+    <t>Onion</t>
+  </si>
+  <si>
+    <t>Currently not included</t>
+  </si>
+  <si>
+    <t>Suru variety</t>
+  </si>
+  <si>
+    <t>Pre-seasonal variety</t>
+  </si>
+  <si>
+    <t>Adsali variety</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">KC# </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>Crop coefficient of growth stage #</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>KY#</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Yield coefficient of growth stage #</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>EM#</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Months since the day of planting to the end of growth stage #</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">modflowWaterLevel, head_development_segments, allowedPumping, gwstorage_cell_avail, areaCrops_Irr_segment[0], areaCrops_Irr_segment[1], areaCrops_Irr_segment[2], areaCrops_Irr_segment[3], areaCrops_Irr_segment[4], areaCrops_Irr_segment[5], areaCrops_Irr_segment[6], areaCrops_Irr_segment[7], areaCrops_Irr_segment[8], areaCrops_Irr_segment[9], areaCrops_Irr_segment[10], areaCrops_Irr_segment[11], areaCrops_Irr_segment[12], areaCrops_Irr_segment[13], areaCrops_Irr_segment[14], areaCrops_Irr_segment[15], fracVegCover[1], fracVegCover[3], frac_totalIrr, frac_totalnonIrr, fracCrops_Irr[0],  fracCrops_Irr[1], fracCrops_Irr[2], fracCrops_Irr[3], fracCrops_Irr[4], fracCrops_Irr[5], fracCrops_Irr[6], fracCrops_Irr[7], fracCrops_Irr[8], fracCrops_Irr[9], fracCrops_Irr[10], fracCrops_Irr[11], fracCrops_Irr[12], fracCrops_Irr[13], fracCrops_Irr[14], fracCrops_Irr[15], fracCrops_nonIrr[0], fracCrops_nonIrr[1], fracCrops_nonIrr[2], fracCrops_nonIrr[3], fracCrops_nonIrr[4], fracCrops_nonIrr[5], fracCrops_nonIrr[6], fracCrops_nonIrr[7],  fracCrops_nonIrr[8], fracCrops_nonIrr[9], fracCrops_nonIrr[10], fracCrops_nonIrr[11], fracCrops_nonIrr[12], fracCrops_nonIrr[13], fracCrops_nonIrr[14], fracCrops_nonIrr[15], fracCrops_IrrLandDemand[0],  fracCrops_IrrLandDemand[1], fracCrops_IrrLandDemand[2], fracCrops_IrrLandDemand[3], fracCrops_IrrLandDemand[4], fracCrops_IrrLandDemand[5], fracCrops_IrrLandDemand[6], fracCrops_IrrLandDemand[7],fracCrops_IrrLandDemand[8], fracCrops_IrrLandDemand[9], fracCrops_IrrLandDemand[10], fracCrops_IrrLandDemand[11], fracCrops_IrrLandDemand[12], fracCrops_IrrLandDemand[13], fracCrops_IrrLandDemand[14], fracCrops_IrrLandDemand[15], fracCrops_nonIrrLandDemand[0],  fracCrops_nonIrrLandDemand[1], fracCrops_nonIrrLandDemand[2], fracCrops_nonIrrLandDemand[3], fracCrops_nonIrrLandDemand[4], fracCrops_nonIrrLandDemand[5], fracCrops_nonIrrLandDemand[6], fracCrops_nonIrrLandDemand[7], fracCrops_nonIrrLandDemand[8], fracCrops_nonIrrLandDemand[9], fracCrops_nonIrrLandDemand[10], fracCrops_nonIrrLandDemand[11], fracCrops_nonIrrLandDemand[12], fracCrops_nonIrrLandDemand[13], fracCrops_nonIrrLandDemand[14], fracCrops_nonIrrLandDemand[15]     </t>
+  </si>
+  <si>
+    <t>Outputs for Taher</t>
+  </si>
+  <si>
+    <t>fracVegCover[3], cropKC[1], cropKC[3], totalPotET[1], totalPotET[3], Yield_Irr[1], Yield_Irr[5], Yield_Irr[7], Yield_Irr[10], Yield_Irr[12], ratio_a_p_Irr[1], ratio_a_p_Irr[5], ratio_a_p_Irr[7],ratio_a_p_Irr[10], ratio_a_p_Irr[12], totalPotET_month_Irr[1], actTransTotal_month_Irr[1]</t>
+  </si>
+  <si>
+    <t>75.89583 17.3875</t>
+  </si>
+  <si>
+    <t>rainAverage_segments, precipEffectiveAverage_segments, precipEffectiveAverage_woBare_segments</t>
+  </si>
+  <si>
+    <t>ratio_a_p_Irr[1], modflowWaterLevel, head_development_segments, allowedPumping, gwstorage_cell_avail, areaCrops_Irr_segment[0], areaCrops_Irr_segment[1], areaCrops_Irr_segment[2], areaCrops_Irr_segment[3], areaCrops_Irr_segment[4], areaCrops_Irr_segment[5], areaCrops_Irr_segment[6], areaCrops_Irr_segment[7], areaCrops_Irr_segment[8], areaCrops_Irr_segment[9], areaCrops_Irr_segment[10], areaCrops_Irr_segment[11], areaCrops_Irr_segment[12], areaCrops_Irr_segment[13], areaCrops_Irr_segment[14], fracVegCover[1], fracVegCover[3], frac_totalIrr, frac_totalnonIrr, fracCrops_Irr[0],  fracCrops_Irr[1], fracCrops_Irr[2], fracCrops_Irr[3], fracCrops_Irr[4], fracCrops_Irr[5], fracCrops_Irr[6], fracCrops_Irr[7], fracCrops_Irr[8], fracCrops_Irr[9], fracCrops_Irr[10], fracCrops_Irr[11], fracCrops_Irr[12], fracCrops_Irr[13], fracCrops_Irr[14], fracCrops_nonIrr[0], fracCrops_nonIrr[1], fracCrops_nonIrr[2], fracCrops_nonIrr[3], fracCrops_nonIrr[4], fracCrops_nonIrr[5], fracCrops_nonIrr[6], fracCrops_nonIrr[7],  fracCrops_nonIrr[8], fracCrops_nonIrr[9], fracCrops_nonIrr[10], fracCrops_nonIrr[11], fracCrops_nonIrr[12], fracCrops_nonIrr[13], fracCrops_nonIrr[14], fracCrops_IrrLandDemand[0],  fracCrops_IrrLandDemand[1], fracCrops_IrrLandDemand[2], fracCrops_IrrLandDemand[3], fracCrops_IrrLandDemand[4], fracCrops_IrrLandDemand[5], fracCrops_IrrLandDemand[6], fracCrops_IrrLandDemand[7],fracCrops_IrrLandDemand[8], fracCrops_IrrLandDemand[9], fracCrops_IrrLandDemand[10], fracCrops_IrrLandDemand[11], fracCrops_IrrLandDemand[12], fracCrops_IrrLandDemand[13], fracCrops_IrrLandDemand[14], fracCrops_nonIrrLandDemand[0],  fracCrops_nonIrrLandDemand[1], fracCrops_nonIrrLandDemand[2], fracCrops_nonIrrLandDemand[3], fracCrops_nonIrrLandDemand[4], fracCrops_nonIrrLandDemand[5], fracCrops_nonIrrLandDemand[6], fracCrops_nonIrrLandDemand[7], fracCrops_nonIrrLandDemand[8], fracCrops_nonIrrLandDemand[9], fracCrops_nonIrrLandDemand[10], fracCrops_nonIrrLandDemand[11], fracCrops_nonIrrLandDemand[12], fracCrops_nonIrrLandDemand[13], fracCrops_nonIrrLandDemand[14], Yield_Irr[1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 01/05/2004</t>
+  </si>
+  <si>
     <t>discharge</t>
   </si>
   <si>
-    <t>, lakeResInflowDis, lakeResOutflowDis, lakeResStorage, act_bigLakeResAbst_alloc, gwstorage_cell_avail, allowedPumping, gwstorage_cell_avail</t>
-  </si>
-  <si>
-    <t>modflowtotalSoilThickness, cellArea, adminSegments_area, adminSegments</t>
-  </si>
-  <si>
-    <t>modflowWaterLevel, areaCrops_Irr_segment[0], areaCrops_Irr_segment[1], areaCrops_Irr_segment[2], areaCrops_Irr_segment[3], areaCrops_Irr_segment[4], areaCrops_Irr_segment[5], areaCrops_Irr_segment[6], areaCrops_Irr_segment[7], head_development_segments, allowedPumping, gwstorage_cell_avail, fracVegCover[1], fracVegCover[3], frac_totalIrr, frac_totalnonIrr, fracCrops_Irr[0],  fracCrops_Irr[1], fracCrops_Irr[2], fracCrops_Irr[3], fracCrops_Irr[4], fracCrops_Irr[5], fracCrops_Irr[6], fracCrops_Irr[7],  fracCrops_nonIrr[0], fracCrops_nonIrr[1], fracCrops_nonIrr[2], fracCrops_nonIrr[3], fracCrops_nonIrr[4], fracCrops_nonIrr[5], fracCrops_nonIrr[6], fracCrops_nonIrr[7],  fracCrops_IrrLandDemand[0],  fracCrops_IrrLandDemand[1], fracCrops_IrrLandDemand[2], fracCrops_IrrLandDemand[3], fracCrops_IrrLandDemand[4], fracCrops_IrrLandDemand[5], fracCrops_IrrLandDemand[6], fracCrops_IrrLandDemand[7], fracCrops_nonIrrLandDemand[0],  fracCrops_nonIrrLandDemand[1], fracCrops_nonIrrLandDemand[2], fracCrops_nonIrrLandDemand[3], fracCrops_nonIrrLandDemand[4], fracCrops_nonIrrLandDemand[5], fracCrops_nonIrrLandDemand[6], fracCrops_nonIrrLandDemand[7], areaCrops_Irr_segment[1], areaCrops_Irr_segment[2]</t>
+    <t xml:space="preserve"> 12/06/2005</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2375,8 +2565,27 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF3644F8"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="26">
+  <fills count="31">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2527,8 +2736,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00A87C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF004835"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF007E5D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF996633"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF960032"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="41">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -3034,11 +3273,89 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF00A87C"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF00A87C"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF00A87C"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF00A87C"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF00A87C"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF00A87C"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF00A87C"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF00A87C"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="186">
+  <cellXfs count="239">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3435,11 +3752,99 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="29" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="29" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="29" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="26" fillId="15" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="26" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="26" fillId="15" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="26" fillId="29" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="26" fillId="29" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="26" fillId="29" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="26" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="26" fillId="15" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="26" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="26" fillId="29" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="26" fillId="29" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="26" fillId="29" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="50">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF636EFA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF636EFA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF636EFA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF636EFA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF636EFA"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3720,22 +4125,6 @@
           <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -3758,13 +4147,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color theme="1" tint="0.499984740745262"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color theme="1" tint="0.499984740745262"/>
         </left>
@@ -3779,18 +4161,43 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="1" tint="0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF00A87C"/>
+      <color rgb="FF996633"/>
+      <color rgb="FF636EFA"/>
+      <color rgb="FF960032"/>
+      <color rgb="FF007E5D"/>
+      <color rgb="FFFF6699"/>
+      <color rgb="FF202FF8"/>
+      <color rgb="FF004835"/>
       <color rgb="FF15FFC2"/>
       <color rgb="FF3644F8"/>
-      <color rgb="FF636EFA"/>
-      <color rgb="FF6699FF"/>
-      <color rgb="FF00966F"/>
-      <color rgb="FF00CC96"/>
-      <color rgb="FF00A87C"/>
-      <color rgb="FF007A5A"/>
     </mruColors>
   </colors>
   <extLst>
@@ -3966,11 +4373,65 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>156210</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>153934</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>826770</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FBE4819-89AE-43D5-A0B7-EE3343B2444C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect t="25604"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="156210" y="336814"/>
+          <a:ext cx="670560" cy="714746"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DCB2946F-7D22-4D9D-A1A7-700B60BA5471}" name="Table3" displayName="Table3" ref="A1:A320" totalsRowShown="0" headerRowDxfId="39" dataDxfId="40" headerRowBorderDxfId="43" tableBorderDxfId="44" totalsRowBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DCB2946F-7D22-4D9D-A1A7-700B60BA5471}" name="Table3" displayName="Table3" ref="A1:A320" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46" totalsRowBorderDxfId="45">
   <autoFilter ref="A1:A320" xr:uid="{899F2FC2-D930-4738-BF7B-C93ECDFC8D39}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{263307C3-FD93-4A08-AAD3-3D1779039680}" name="Column1" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{263307C3-FD93-4A08-AAD3-3D1779039680}" name="Column1" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4276,10 +4737,10 @@
   <sheetPr>
     <tabColor rgb="FF636EFA"/>
   </sheetPr>
-  <dimension ref="A1:J57"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4321,7 +4782,7 @@
         <v>123</v>
       </c>
       <c r="B2" s="181" t="s">
-        <v>712</v>
+        <v>760</v>
       </c>
       <c r="F2" s="107" t="s">
         <v>619</v>
@@ -4332,8 +4793,11 @@
       <c r="A3" s="104" t="s">
         <v>124</v>
       </c>
-      <c r="B3" s="169" t="s">
+      <c r="B3" s="181" t="s">
         <v>9</v>
+      </c>
+      <c r="D3" s="169" t="s">
+        <v>741</v>
       </c>
       <c r="F3" s="107" t="s">
         <v>578</v>
@@ -4347,10 +4811,13 @@
         <v>126</v>
       </c>
       <c r="B4" s="181" t="s">
-        <v>713</v>
+        <v>762</v>
       </c>
       <c r="D4" s="181" t="s">
-        <v>713</v>
+        <v>710</v>
+      </c>
+      <c r="E4" s="181" t="s">
+        <v>742</v>
       </c>
       <c r="F4" s="107" t="s">
         <v>622</v>
@@ -4364,7 +4831,7 @@
         <v>407</v>
       </c>
       <c r="B5" s="169">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="F5" s="93"/>
       <c r="G5" s="100"/>
@@ -4379,7 +4846,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="112" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="F6" s="93" t="s">
         <v>630</v>
@@ -4391,7 +4858,7 @@
         <v>544</v>
       </c>
       <c r="B7" s="169" t="s">
-        <v>714</v>
+        <v>761</v>
       </c>
       <c r="D7" s="112" t="s">
         <v>685</v>
@@ -4408,18 +4875,10 @@
       <c r="A8" s="104" t="s">
         <v>517</v>
       </c>
-      <c r="B8" s="169" t="s">
-        <v>717</v>
-      </c>
-      <c r="D8" s="112" t="s">
-        <v>707</v>
-      </c>
-      <c r="E8" s="117" t="s">
-        <v>678</v>
-      </c>
-      <c r="F8" s="93" t="s">
-        <v>631</v>
-      </c>
+      <c r="B8" s="235" t="s">
+        <v>759</v>
+      </c>
+      <c r="F8" s="93"/>
       <c r="G8" s="100"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -4427,7 +4886,7 @@
         <v>561</v>
       </c>
       <c r="B9" s="170" t="s">
-        <v>709</v>
+        <v>758</v>
       </c>
       <c r="F9" s="93"/>
       <c r="G9" s="100"/>
@@ -4437,10 +4896,10 @@
         <v>695</v>
       </c>
       <c r="B10" s="170" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="D10" s="112" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="F10" s="93"/>
       <c r="G10" s="100"/>
@@ -4458,6 +4917,9 @@
         <v>563</v>
       </c>
       <c r="B12" s="169"/>
+      <c r="D12" s="112" t="s">
+        <v>756</v>
+      </c>
       <c r="F12" s="93"/>
       <c r="G12" s="100"/>
     </row>
@@ -4466,7 +4928,7 @@
         <v>564</v>
       </c>
       <c r="B13" s="171" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="C13" s="95"/>
       <c r="D13" s="113"/>
@@ -4506,7 +4968,7 @@
       <c r="F16" s="93"/>
       <c r="G16" s="100"/>
     </row>
-    <row r="17" spans="1:10" s="144" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:8" s="144" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="141" t="s">
         <v>117</v>
       </c>
@@ -4518,378 +4980,382 @@
       <c r="E17" s="142"/>
       <c r="F17" s="143"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="182" t="s">
-        <v>79</v>
-      </c>
-      <c r="B18" s="169" t="b">
+    <row r="18" spans="1:8" s="144" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="141" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" s="172" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="142"/>
+      <c r="D18" s="142"/>
+      <c r="E18" s="142"/>
+      <c r="F18" s="143"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="104" t="s">
+        <v>127</v>
+      </c>
+      <c r="B19" s="169" t="b">
         <v>1</v>
       </c>
-      <c r="D18" s="112" t="b">
+      <c r="F19" s="93"/>
+      <c r="G19" s="100"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="182" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="107" t="s">
+        <v>640</v>
+      </c>
+      <c r="D20" s="107" t="s">
+        <v>723</v>
+      </c>
+      <c r="E20" s="107" t="s">
+        <v>640</v>
+      </c>
+      <c r="F20" s="107" t="s">
+        <v>684</v>
+      </c>
+      <c r="G20" s="100"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="104" t="s">
+        <v>129</v>
+      </c>
+      <c r="B21" s="169" t="b">
         <v>0</v>
       </c>
-      <c r="F18" s="93"/>
-      <c r="G18" s="100"/>
-    </row>
-    <row r="19" spans="1:10" s="144" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="141" t="s">
-        <v>105</v>
-      </c>
-      <c r="B19" s="172" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="142"/>
-      <c r="D19" s="142"/>
-      <c r="E19" s="142"/>
-      <c r="F19" s="143"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="104" t="s">
-        <v>127</v>
-      </c>
-      <c r="B20" s="169" t="b">
-        <v>1</v>
-      </c>
-      <c r="F20" s="93"/>
-      <c r="G20" s="100"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="182" t="s">
-        <v>128</v>
-      </c>
-      <c r="B21" s="107" t="s">
-        <v>640</v>
-      </c>
-      <c r="D21" s="107" t="s">
-        <v>687</v>
-      </c>
-      <c r="E21" s="107" t="s">
-        <v>640</v>
-      </c>
-      <c r="F21" s="107" t="s">
-        <v>684</v>
+      <c r="F21" s="93" t="s">
+        <v>537</v>
       </c>
       <c r="G21" s="100"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="104" t="s">
-        <v>129</v>
-      </c>
-      <c r="B22" s="169" t="b">
-        <v>0</v>
-      </c>
-      <c r="F22" s="93" t="s">
-        <v>537</v>
-      </c>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="182" t="s">
+        <v>130</v>
+      </c>
+      <c r="B22" s="183" t="s">
+        <v>559</v>
+      </c>
+      <c r="D22" s="112" t="s">
+        <v>635</v>
+      </c>
+      <c r="E22" s="117" t="s">
+        <v>634</v>
+      </c>
+      <c r="F22" s="93"/>
       <c r="G22" s="100"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="182" t="s">
-        <v>130</v>
-      </c>
-      <c r="B23" s="183" t="s">
-        <v>706</v>
-      </c>
-      <c r="D23" s="112" t="s">
-        <v>635</v>
-      </c>
-      <c r="E23" s="117" t="s">
-        <v>634</v>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="104" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" s="181" t="s">
+        <v>762</v>
       </c>
       <c r="F23" s="93"/>
       <c r="G23" s="100"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="104" t="s">
-        <v>131</v>
-      </c>
-      <c r="B24" s="169" t="s">
-        <v>683</v>
+        <v>390</v>
+      </c>
+      <c r="B24" s="169" t="b">
+        <v>0</v>
       </c>
       <c r="F24" s="93"/>
       <c r="G24" s="100"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="104" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B25" s="169" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E25" s="117" t="s">
+        <v>641</v>
       </c>
       <c r="F25" s="93"/>
       <c r="G25" s="100"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="H25" s="98"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="104" t="s">
-        <v>391</v>
-      </c>
-      <c r="B26" s="169" t="b">
-        <v>1</v>
-      </c>
-      <c r="E26" s="117" t="s">
-        <v>641</v>
-      </c>
-      <c r="F26" s="93"/>
-      <c r="G26" s="100"/>
-      <c r="H26" s="98"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="104" t="s">
-        <v>171</v>
-      </c>
-      <c r="B27" s="169" t="s">
-        <v>638</v>
-      </c>
-      <c r="C27" s="96"/>
-      <c r="D27" s="114"/>
-      <c r="E27" s="119"/>
-      <c r="F27" s="94" t="s">
-        <v>621</v>
-      </c>
-      <c r="G27" s="101"/>
-      <c r="H27" s="99"/>
-      <c r="I27" s="87"/>
-      <c r="J27" s="88"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="104" t="s">
-        <v>173</v>
-      </c>
-      <c r="B28" s="169" t="s">
-        <v>639</v>
-      </c>
-      <c r="C28" s="97"/>
-      <c r="D28" s="115"/>
-      <c r="E28" s="120"/>
-      <c r="F28" s="93" t="s">
-        <v>620</v>
-      </c>
-      <c r="G28" s="102"/>
-      <c r="H28" s="98"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="104" t="s">
         <v>277</v>
       </c>
-      <c r="B29" s="169" t="s">
+      <c r="B26" s="169" t="s">
         <v>278</v>
       </c>
-      <c r="F29" s="93">
+      <c r="F26" s="93">
         <f>0.00003*24*60*60</f>
         <v>2.5920000000000001</v>
       </c>
+      <c r="G26" s="100"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="104" t="s">
+        <v>269</v>
+      </c>
+      <c r="B27" s="169" t="s">
+        <v>270</v>
+      </c>
+      <c r="F27" s="93"/>
+      <c r="G27" s="100"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="182" t="s">
+        <v>118</v>
+      </c>
+      <c r="B28" s="169" t="s">
+        <v>629</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E28" s="169" t="s">
+        <v>629</v>
+      </c>
+      <c r="F28" s="93"/>
+      <c r="G28" s="100"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="103" t="s">
+        <v>603</v>
+      </c>
+      <c r="B29" s="169" t="s">
+        <v>604</v>
+      </c>
+      <c r="F29" s="93"/>
       <c r="G29" s="100"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="104" t="s">
-        <v>269</v>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="103" t="s">
+        <v>586</v>
       </c>
       <c r="B30" s="169" t="s">
-        <v>270</v>
+        <v>716</v>
       </c>
       <c r="F30" s="93"/>
       <c r="G30" s="100"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="182" t="s">
-        <v>118</v>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="103" t="s">
+        <v>610</v>
       </c>
       <c r="B31" s="169" t="s">
-        <v>629</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>119</v>
+        <v>716</v>
       </c>
       <c r="F31" s="93"/>
       <c r="G31" s="100"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="103" t="s">
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="B32" s="169" t="s">
-        <v>604</v>
+        <v>716</v>
       </c>
       <c r="F32" s="93"/>
       <c r="G32" s="100"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="103" t="s">
-        <v>586</v>
+        <v>612</v>
       </c>
       <c r="B33" s="169" t="s">
-        <v>605</v>
+        <v>716</v>
+      </c>
+      <c r="D33" s="169" t="s">
+        <v>715</v>
       </c>
       <c r="F33" s="93"/>
       <c r="G33" s="100"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="103" t="s">
-        <v>610</v>
+        <v>583</v>
       </c>
       <c r="B34" s="169" t="s">
-        <v>605</v>
+        <v>717</v>
       </c>
       <c r="F34" s="93"/>
       <c r="G34" s="100"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="103" t="s">
-        <v>611</v>
+        <v>584</v>
       </c>
       <c r="B35" s="169" t="s">
-        <v>605</v>
+        <v>718</v>
       </c>
       <c r="F35" s="93"/>
       <c r="G35" s="100"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="103" t="s">
-        <v>612</v>
+        <v>585</v>
       </c>
       <c r="B36" s="169" t="s">
-        <v>605</v>
+        <v>719</v>
       </c>
       <c r="F36" s="93"/>
       <c r="G36" s="100"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A37" s="103" t="s">
-        <v>583</v>
-      </c>
-      <c r="B37" s="169" t="s">
-        <v>607</v>
+        <v>588</v>
+      </c>
+      <c r="B37" s="173" t="s">
+        <v>720</v>
       </c>
       <c r="F37" s="93"/>
       <c r="G37" s="100"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="103" t="s">
-        <v>584</v>
-      </c>
-      <c r="B38" s="169" t="s">
-        <v>608</v>
-      </c>
-      <c r="F38" s="93"/>
-      <c r="G38" s="100"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="103" t="s">
-        <v>585</v>
-      </c>
-      <c r="B39" s="169" t="s">
-        <v>609</v>
-      </c>
-      <c r="F39" s="93"/>
-      <c r="G39" s="100"/>
-    </row>
-    <row r="40" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A40" s="103" t="s">
-        <v>588</v>
-      </c>
-      <c r="B40" s="173" t="s">
-        <v>606</v>
-      </c>
-      <c r="F40" s="93"/>
-      <c r="G40" s="100"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="15" t="s">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="15" t="s">
         <v>547</v>
       </c>
-      <c r="B41" s="174" t="s">
+      <c r="B38" s="174" t="s">
         <v>624</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="184" t="s">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="184" t="s">
         <v>120</v>
       </c>
-      <c r="B42" s="9" t="s">
-        <v>633</v>
-      </c>
-      <c r="D42" s="112" t="s">
-        <v>647</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="7" t="s">
+      <c r="B39" s="9" t="s">
+        <v>757</v>
+      </c>
+      <c r="D39" s="112" t="s">
+        <v>722</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="184" t="s">
         <v>387</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B40" s="9" t="s">
         <v>632</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="D40" s="9" t="s">
         <v>645</v>
       </c>
-      <c r="E43" s="9" t="s">
+      <c r="E40" s="9" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="185" t="s">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="185" t="s">
         <v>636</v>
       </c>
-      <c r="B44" s="90" t="s">
+      <c r="B41" s="90" t="s">
         <v>642</v>
       </c>
-      <c r="D44" s="112" t="s">
+      <c r="D41" s="112" t="s">
         <v>637</v>
       </c>
-      <c r="E44" s="90" t="s">
+      <c r="E41" s="90" t="s">
         <v>642</v>
       </c>
-      <c r="F44" s="112" t="s">
+      <c r="F41" s="112" t="s">
         <v>648</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="7" t="s">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="7" t="s">
         <v>466</v>
       </c>
-      <c r="B45" s="175">
+      <c r="B42" s="175">
         <v>160</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="7" t="s">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="184" t="s">
         <v>17</v>
       </c>
-      <c r="B46" s="112" t="s">
+      <c r="B43" s="112" t="s">
         <v>18</v>
       </c>
-      <c r="D46" s="112" t="s">
+      <c r="D43" s="112" t="s">
         <v>18</v>
       </c>
-      <c r="E46" s="90" t="s">
+      <c r="E43" s="90" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="144" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="144" t="s">
+    <row r="44" spans="1:10" s="144" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="144" t="s">
         <v>651</v>
       </c>
-      <c r="B47" s="178" t="b">
+      <c r="B44" s="178" t="b">
         <v>1</v>
       </c>
-      <c r="C47" s="142"/>
-      <c r="D47" s="142"/>
-      <c r="E47" s="142"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="139" t="s">
+      <c r="C44" s="142"/>
+      <c r="D44" s="142"/>
+      <c r="E44" s="142"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="139" t="s">
         <v>676</v>
       </c>
-      <c r="B48" s="179">
+      <c r="B45" s="179">
         <v>1</v>
       </c>
     </row>
+    <row r="46" spans="1:10" s="91" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="139" t="s">
+        <v>680</v>
+      </c>
+      <c r="B46" s="179">
+        <v>1</v>
+      </c>
+      <c r="D46" s="112"/>
+      <c r="E46" s="117"/>
+      <c r="F46" s="83"/>
+      <c r="G46" s="83"/>
+      <c r="H46" s="83"/>
+      <c r="I46" s="83"/>
+      <c r="J46" s="83"/>
+    </row>
+    <row r="47" spans="1:10" s="91" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="83" t="s">
+        <v>681</v>
+      </c>
+      <c r="B47" s="179">
+        <v>1</v>
+      </c>
+      <c r="D47" s="112"/>
+      <c r="E47" s="117"/>
+      <c r="F47" s="83"/>
+      <c r="G47" s="83"/>
+      <c r="H47" s="83"/>
+      <c r="I47" s="83"/>
+      <c r="J47" s="83"/>
+    </row>
+    <row r="48" spans="1:10" s="91" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B48" s="179" t="b">
+        <v>1</v>
+      </c>
+      <c r="D48" s="112"/>
+      <c r="E48" s="117"/>
+      <c r="F48" s="83"/>
+      <c r="G48" s="83"/>
+      <c r="H48" s="83"/>
+      <c r="I48" s="83"/>
+      <c r="J48" s="83"/>
+    </row>
     <row r="49" spans="1:10" s="91" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="139" t="s">
-        <v>680</v>
+      <c r="A49" s="140" t="s">
+        <v>682</v>
       </c>
       <c r="B49" s="179">
         <v>1</v>
@@ -4903,11 +5369,11 @@
       <c r="J49" s="83"/>
     </row>
     <row r="50" spans="1:10" s="91" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="83" t="s">
-        <v>681</v>
-      </c>
-      <c r="B50" s="179">
-        <v>0.5</v>
+      <c r="A50" s="7" t="s">
+        <v>701</v>
+      </c>
+      <c r="B50" s="180">
+        <v>1</v>
       </c>
       <c r="D50" s="112"/>
       <c r="E50" s="117"/>
@@ -4919,9 +5385,9 @@
     </row>
     <row r="51" spans="1:10" s="91" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B51" s="179" t="b">
+        <v>702</v>
+      </c>
+      <c r="B51" s="180">
         <v>1</v>
       </c>
       <c r="D51" s="112"/>
@@ -4933,8 +5399,8 @@
       <c r="J51" s="83"/>
     </row>
     <row r="52" spans="1:10" s="91" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="140" t="s">
-        <v>682</v>
+      <c r="A52" s="83" t="s">
+        <v>703</v>
       </c>
       <c r="B52" s="179">
         <v>1</v>
@@ -4947,132 +5413,223 @@
       <c r="I52" s="83"/>
       <c r="J52" s="83"/>
     </row>
-    <row r="53" spans="1:10" s="91" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="7" t="s">
-        <v>701</v>
-      </c>
-      <c r="B53" s="180">
-        <v>1</v>
-      </c>
-      <c r="D53" s="112"/>
-      <c r="E53" s="117"/>
-      <c r="F53" s="83"/>
-      <c r="G53" s="83"/>
-      <c r="H53" s="83"/>
-      <c r="I53" s="83"/>
-      <c r="J53" s="83"/>
-    </row>
-    <row r="54" spans="1:10" s="91" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="7" t="s">
-        <v>702</v>
-      </c>
-      <c r="B54" s="180">
-        <v>1</v>
-      </c>
-      <c r="D54" s="112"/>
-      <c r="E54" s="117"/>
-      <c r="F54" s="83"/>
-      <c r="G54" s="83"/>
-      <c r="H54" s="83"/>
-      <c r="I54" s="83"/>
-      <c r="J54" s="83"/>
-    </row>
-    <row r="55" spans="1:10" s="91" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="83" t="s">
-        <v>703</v>
-      </c>
-      <c r="B55" s="179">
-        <v>1</v>
-      </c>
-      <c r="D55" s="112"/>
-      <c r="E55" s="117"/>
-      <c r="F55" s="83"/>
-      <c r="G55" s="83"/>
-      <c r="H55" s="83"/>
-      <c r="I55" s="83"/>
-      <c r="J55" s="83"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="147" t="s">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="147" t="s">
         <v>425</v>
       </c>
-      <c r="B56" s="148" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="147" t="s">
+      <c r="B53" s="148" t="s">
+        <v>744</v>
+      </c>
+      <c r="D53" s="148" t="s">
+        <v>706</v>
+      </c>
+      <c r="E53" s="117" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="147" t="s">
         <v>540</v>
       </c>
-      <c r="B57" s="148" t="s">
+      <c r="B54" s="148" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="145" t="s">
+        <v>712</v>
+      </c>
+      <c r="B55" s="112">
+        <v>0.5</v>
+      </c>
+      <c r="D55" s="112" t="s">
+        <v>714</v>
+      </c>
+      <c r="E55" s="112" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A56" s="49" t="s">
+        <v>729</v>
+      </c>
+      <c r="B56" s="173" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A57" s="49" t="s">
+        <v>730</v>
+      </c>
+      <c r="B57" s="173" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A58" s="49" t="s">
+        <v>731</v>
+      </c>
+      <c r="B58" s="173" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A59" s="49" t="s">
+        <v>732</v>
+      </c>
+      <c r="B59" s="173" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A60" s="49" t="s">
+        <v>725</v>
+      </c>
+      <c r="B60" s="173" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A61" s="49" t="s">
+        <v>727</v>
+      </c>
+      <c r="B61" s="173" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A62" s="83" t="s">
+        <v>728</v>
+      </c>
+      <c r="B62" s="173" t="s">
+        <v>734</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <conditionalFormatting sqref="B5:B20 B25:B40 B22:B23">
-    <cfRule type="notContainsErrors" dxfId="38" priority="25">
-      <formula>NOT(ISERROR(B5))</formula>
+  <conditionalFormatting sqref="B21:B22 B29:B37 B5:B7 D3 B24:B27 B11:B19">
+    <cfRule type="notContainsErrors" dxfId="43" priority="65">
+      <formula>NOT(ISERROR(B3))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="notContainsErrors" dxfId="37" priority="24">
+    <cfRule type="notContainsErrors" dxfId="42" priority="64">
       <formula>NOT(ISERROR(F4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="notContainsErrors" dxfId="36" priority="23">
+    <cfRule type="notContainsErrors" dxfId="41" priority="63">
       <formula>NOT(ISERROR(F2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="notContainsErrors" dxfId="35" priority="22">
+    <cfRule type="notContainsErrors" dxfId="40" priority="62">
       <formula>NOT(ISERROR(F3))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F21">
-    <cfRule type="notContainsErrors" dxfId="34" priority="21">
-      <formula>NOT(ISERROR(F21))</formula>
+  <conditionalFormatting sqref="F20">
+    <cfRule type="notContainsErrors" dxfId="39" priority="61">
+      <formula>NOT(ISERROR(F20))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
-    <cfRule type="notContainsErrors" dxfId="33" priority="20">
-      <formula>NOT(ISERROR(E21))</formula>
+  <conditionalFormatting sqref="E20">
+    <cfRule type="notContainsErrors" dxfId="38" priority="60">
+      <formula>NOT(ISERROR(E20))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D21">
-    <cfRule type="notContainsErrors" dxfId="32" priority="19">
-      <formula>NOT(ISERROR(D21))</formula>
+  <conditionalFormatting sqref="D20">
+    <cfRule type="notContainsErrors" dxfId="37" priority="59">
+      <formula>NOT(ISERROR(D20))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B24">
-    <cfRule type="notContainsErrors" dxfId="30" priority="17">
-      <formula>NOT(ISERROR(B24))</formula>
+  <conditionalFormatting sqref="D4">
+    <cfRule type="notContainsErrors" dxfId="36" priority="42">
+      <formula>NOT(ISERROR(D4))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="notContainsErrors" dxfId="33" priority="35">
+      <formula>NOT(ISERROR(B2))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33">
+    <cfRule type="notContainsErrors" dxfId="32" priority="33">
+      <formula>NOT(ISERROR(D33))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="notContainsErrors" dxfId="31" priority="32">
+      <formula>NOT(ISERROR(E28))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B58">
+    <cfRule type="notContainsErrors" dxfId="30" priority="20">
+      <formula>NOT(ISERROR(B58))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B56">
+    <cfRule type="notContainsErrors" dxfId="29" priority="18">
+      <formula>NOT(ISERROR(B56))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B62">
+    <cfRule type="notContainsErrors" dxfId="28" priority="24">
+      <formula>NOT(ISERROR(B62))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B61">
+    <cfRule type="notContainsErrors" dxfId="27" priority="23">
+      <formula>NOT(ISERROR(B61))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B60">
+    <cfRule type="notContainsErrors" dxfId="26" priority="22">
+      <formula>NOT(ISERROR(B60))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B59">
+    <cfRule type="notContainsErrors" dxfId="25" priority="21">
+      <formula>NOT(ISERROR(B59))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B57">
+    <cfRule type="notContainsErrors" dxfId="24" priority="19">
+      <formula>NOT(ISERROR(B57))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="notContainsErrors" dxfId="22" priority="13">
+      <formula>NOT(ISERROR(E4))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:B10">
+    <cfRule type="notContainsErrors" dxfId="5" priority="6">
+      <formula>NOT(ISERROR(B9))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20">
+    <cfRule type="notContainsErrors" dxfId="4" priority="5">
+      <formula>NOT(ISERROR(B20))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28">
+    <cfRule type="notContainsErrors" dxfId="3" priority="4">
+      <formula>NOT(ISERROR(B28))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4">
+    <cfRule type="notContainsErrors" dxfId="2" priority="3">
+      <formula>NOT(ISERROR(B4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="notContainsErrors" dxfId="29" priority="14">
+    <cfRule type="notContainsErrors" dxfId="1" priority="2">
       <formula>NOT(ISERROR(B3))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="notContainsErrors" dxfId="28" priority="15">
-      <formula>NOT(ISERROR(B2))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21">
-    <cfRule type="notContainsErrors" dxfId="26" priority="13">
-      <formula>NOT(ISERROR(B21))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D4">
-    <cfRule type="notContainsErrors" dxfId="1" priority="2">
-      <formula>NOT(ISERROR(D4))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4">
+  <conditionalFormatting sqref="B23">
     <cfRule type="notContainsErrors" dxfId="0" priority="1">
-      <formula>NOT(ISERROR(B4))</formula>
+      <formula>NOT(ISERROR(B23))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5082,6 +5639,468 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811BB740-2696-4061-9D1F-96ECA011A915}">
+  <dimension ref="A1:G40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="21.3125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="25.62890625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="1.734375" style="23" customWidth="1"/>
+    <col min="4" max="4" width="73" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83984375" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.3" x14ac:dyDescent="0.7">
+      <c r="A1" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>578</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="42" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2" s="32"/>
+    </row>
+    <row r="3" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A3" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="26"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" s="42">
+        <v>10</v>
+      </c>
+      <c r="C4" s="38"/>
+      <c r="D4" s="33" t="s">
+        <v>566</v>
+      </c>
+      <c r="E4" s="32"/>
+      <c r="F4" s="22" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="41" t="s">
+        <v>407</v>
+      </c>
+      <c r="B5" s="42">
+        <v>1</v>
+      </c>
+      <c r="C5" s="26"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="41" t="s">
+        <v>557</v>
+      </c>
+      <c r="B6" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="26"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="41" t="s">
+        <v>544</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>582</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="32"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="41" t="s">
+        <v>517</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>571</v>
+      </c>
+      <c r="C8" s="26"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="41" t="s">
+        <v>561</v>
+      </c>
+      <c r="B9" s="42"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="41" t="s">
+        <v>562</v>
+      </c>
+      <c r="B10" s="42"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="41" t="s">
+        <v>563</v>
+      </c>
+      <c r="B11" s="42"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="41" t="s">
+        <v>564</v>
+      </c>
+      <c r="B12" s="43" t="s">
+        <v>565</v>
+      </c>
+      <c r="C12" s="27"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="42" t="s">
+        <v>532</v>
+      </c>
+      <c r="C13" s="26"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14" s="42" t="s">
+        <v>533</v>
+      </c>
+      <c r="C14" s="26"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="C15" s="26"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>560</v>
+      </c>
+      <c r="C16" s="26"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="26"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="26"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="26"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>568</v>
+      </c>
+      <c r="C20" s="28"/>
+      <c r="D20" s="35" t="s">
+        <v>558</v>
+      </c>
+      <c r="E20" s="32"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="B21" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="C21" s="26"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+    </row>
+    <row r="22" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A22" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="B22" s="42" t="s">
+        <v>559</v>
+      </c>
+      <c r="C22" s="26"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" s="33" t="s">
+        <v>567</v>
+      </c>
+      <c r="C23" s="26"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="44" t="s">
+        <v>390</v>
+      </c>
+      <c r="B24" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="C24" s="29"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="44" t="s">
+        <v>391</v>
+      </c>
+      <c r="B25" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="C25" s="29"/>
+      <c r="D25" s="32" t="s">
+        <v>572</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>573</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>574</v>
+      </c>
+      <c r="G25" s="21" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="B26" s="45">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C26" s="30"/>
+      <c r="D26" s="36">
+        <v>8.0484411999999994E-6</v>
+      </c>
+      <c r="E26" s="36">
+        <v>3.0484411999999999E-6</v>
+      </c>
+      <c r="F26" s="24">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="G26" s="24">
+        <v>2.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="44" t="s">
+        <v>551</v>
+      </c>
+      <c r="B27" s="46">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C27" s="31"/>
+      <c r="D27" s="32">
+        <v>0.01</v>
+      </c>
+      <c r="E27" s="37">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="F27" s="21">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G27" s="21">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="B28" s="42" t="s">
+        <v>569</v>
+      </c>
+      <c r="C28" s="29"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="B29" s="42" t="s">
+        <v>570</v>
+      </c>
+      <c r="C29" s="29"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="C30" s="29"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="C31" s="29"/>
+      <c r="E31" s="32"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C32" s="29"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="47"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="47"/>
+      <c r="B34" s="42"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="47"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="47"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="47"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="47"/>
+      <c r="B38" s="42"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="47"/>
+      <c r="B39" s="42"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="47"/>
+      <c r="B40" s="42"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB470B68-06CF-4878-82CF-51FDF4D94B75}">
   <dimension ref="A1:G10"/>
   <sheetViews>
@@ -5301,7 +6320,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAC21375-A8E9-4EF5-B764-254BB08A3B84}">
   <dimension ref="A1:B320"/>
   <sheetViews>
@@ -8546,67 +9565,67 @@
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="B5:B19 B24:B39 B21:B22">
-    <cfRule type="notContainsErrors" dxfId="23" priority="14">
+    <cfRule type="notContainsErrors" dxfId="19" priority="14">
       <formula>NOT(ISERROR(B5))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="notContainsErrors" dxfId="22" priority="13">
+    <cfRule type="notContainsErrors" dxfId="18" priority="13">
       <formula>NOT(ISERROR(F4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="notContainsErrors" dxfId="21" priority="12">
+    <cfRule type="notContainsErrors" dxfId="17" priority="12">
       <formula>NOT(ISERROR(F2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="notContainsErrors" dxfId="20" priority="11">
+    <cfRule type="notContainsErrors" dxfId="16" priority="11">
       <formula>NOT(ISERROR(F3))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="notContainsErrors" dxfId="19" priority="10">
+    <cfRule type="notContainsErrors" dxfId="15" priority="10">
       <formula>NOT(ISERROR(F20))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="notContainsErrors" dxfId="18" priority="9">
+    <cfRule type="notContainsErrors" dxfId="14" priority="9">
       <formula>NOT(ISERROR(E20))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="notContainsErrors" dxfId="17" priority="6">
+    <cfRule type="notContainsErrors" dxfId="13" priority="6">
       <formula>NOT(ISERROR(D4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="notContainsErrors" dxfId="16" priority="8">
+    <cfRule type="notContainsErrors" dxfId="12" priority="8">
       <formula>NOT(ISERROR(D20))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="notContainsErrors" dxfId="14" priority="5">
+    <cfRule type="notContainsErrors" dxfId="11" priority="5">
       <formula>NOT(ISERROR(B23))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="notContainsErrors" dxfId="13" priority="4">
+    <cfRule type="notContainsErrors" dxfId="10" priority="4">
       <formula>NOT(ISERROR(B4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="notContainsErrors" dxfId="12" priority="3">
+    <cfRule type="notContainsErrors" dxfId="9" priority="3">
       <formula>NOT(ISERROR(B2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="notContainsErrors" dxfId="11" priority="2">
+    <cfRule type="notContainsErrors" dxfId="8" priority="2">
       <formula>NOT(ISERROR(B3))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="notContainsErrors" dxfId="10" priority="1">
+    <cfRule type="notContainsErrors" dxfId="7" priority="1">
       <formula>NOT(ISERROR(B20))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8621,10 +9640,10 @@
   <sheetPr>
     <tabColor rgb="FF636EFA"/>
   </sheetPr>
-  <dimension ref="A1:F321"/>
+  <dimension ref="A1:F323"/>
   <sheetViews>
-    <sheetView topLeftCell="A308" workbookViewId="0">
-      <selection activeCell="A233" sqref="A233"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -10736,63 +11755,63 @@
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A263" s="145" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="B263" s="146">
         <v>1</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A264" s="147" t="s">
-        <v>451</v>
-      </c>
-      <c r="B264" s="148" t="s">
-        <v>452</v>
+      <c r="A264" s="145" t="s">
+        <v>712</v>
+      </c>
+      <c r="B264" s="146">
+        <v>1</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A265" s="147" t="s">
-        <v>453</v>
-      </c>
-      <c r="B265" s="148" t="s">
-        <v>454</v>
+      <c r="A265" s="145" t="s">
+        <v>680</v>
+      </c>
+      <c r="B265" s="146">
+        <v>1</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A266" s="147" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="B266" s="148" t="s">
-        <v>77</v>
+        <v>452</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A267" s="147" t="s">
-        <v>456</v>
-      </c>
-      <c r="B267" s="148">
-        <v>1</v>
+        <v>453</v>
+      </c>
+      <c r="B267" s="148" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A268" s="147" t="s">
-        <v>457</v>
-      </c>
-      <c r="B268" s="148">
-        <v>0.5</v>
+        <v>455</v>
+      </c>
+      <c r="B268" s="148" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A269" s="147" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B269" s="148">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A270" s="147" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B270" s="148">
         <v>0.5</v>
@@ -10800,397 +11819,413 @@
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A271" s="147" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B271" s="148">
-        <v>0.15</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A272" s="147" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B272" s="148">
-        <v>0.01</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A273" s="147" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B273" s="148">
-        <v>1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A274" s="147" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B274" s="148">
-        <v>2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A275" s="147" t="s">
-        <v>464</v>
-      </c>
-      <c r="B275" s="148" t="s">
-        <v>465</v>
+        <v>462</v>
+      </c>
+      <c r="B275" s="148">
+        <v>1</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A276" s="147" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="B276" s="148">
-        <v>160</v>
+        <v>2</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A277" s="147" t="s">
-        <v>467</v>
-      </c>
-      <c r="B277" s="148">
-        <v>0.6</v>
+        <v>464</v>
+      </c>
+      <c r="B277" s="148" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A278" s="147" t="s">
-        <v>468</v>
-      </c>
-      <c r="B278" s="148" t="s">
-        <v>469</v>
+        <v>466</v>
+      </c>
+      <c r="B278" s="148">
+        <v>160</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A279" s="147" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="B279" s="148">
-        <v>1E-4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A280" s="147" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="B280" s="148" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A281" s="147" t="s">
-        <v>473</v>
-      </c>
-      <c r="B281" s="148" t="s">
-        <v>474</v>
+        <v>470</v>
+      </c>
+      <c r="B281" s="148">
+        <v>1E-4</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A282" s="147" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="B282" s="148" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A283" s="147" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="B283" s="148" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A284" s="147" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="B284" s="148" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A285" s="147" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="B285" s="148" t="s">
-        <v>77</v>
+        <v>478</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A286" s="147" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B286" s="148" t="s">
-        <v>77</v>
+        <v>480</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A287" s="147" t="s">
-        <v>483</v>
-      </c>
-      <c r="B287" s="148">
-        <v>1961</v>
+        <v>481</v>
+      </c>
+      <c r="B287" s="148" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A288" s="147" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B288" s="148" t="s">
-        <v>485</v>
+        <v>77</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A289" s="147" t="s">
-        <v>486</v>
-      </c>
-      <c r="B289" s="148" t="s">
-        <v>487</v>
+        <v>483</v>
+      </c>
+      <c r="B289" s="148">
+        <v>1961</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A290" s="147" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="B290" s="148" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A291" s="147" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="B291" s="148" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A292" s="147" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="B292" s="148" t="s">
-        <v>85</v>
+        <v>489</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A293" s="147" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B293" s="148" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A294" s="147" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B294" s="148" t="s">
-        <v>496</v>
+        <v>85</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A295" s="147" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="B295" s="148" t="s">
-        <v>543</v>
+        <v>494</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A296" s="147" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B296" s="148" t="s">
-        <v>542</v>
+        <v>496</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A297" s="147" t="s">
-        <v>499</v>
-      </c>
-      <c r="B297" s="148">
-        <v>0.02</v>
+        <v>497</v>
+      </c>
+      <c r="B297" s="148" t="s">
+        <v>543</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A298" s="147" t="s">
-        <v>500</v>
-      </c>
-      <c r="B298" s="148">
-        <v>0.9</v>
+        <v>498</v>
+      </c>
+      <c r="B298" s="148" t="s">
+        <v>542</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A299" s="147" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B299" s="148">
-        <v>0.5</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A300" s="147" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B300" s="148">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A301" s="147" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B301" s="148">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A302" s="147" t="s">
+        <v>502</v>
+      </c>
+      <c r="B302" s="148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A303" s="147" t="s">
+        <v>503</v>
+      </c>
+      <c r="B303" s="148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A304" s="147" t="s">
         <v>504</v>
       </c>
-      <c r="B302" s="148">
+      <c r="B304" s="148">
         <v>4</v>
-      </c>
-    </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A303" s="145" t="s">
-        <v>108</v>
-      </c>
-      <c r="B303" s="146" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A304" s="145" t="s">
-        <v>110</v>
-      </c>
-      <c r="B304" s="146">
-        <v>0.92969999999999997</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A305" s="145" t="s">
-        <v>111</v>
-      </c>
-      <c r="B305" s="146">
-        <v>0.94969999999999999</v>
+        <v>108</v>
+      </c>
+      <c r="B305" s="146" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A306" s="145" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B306" s="146">
-        <v>0.98499999999999999</v>
+        <v>0.92969999999999997</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A307" s="145" t="s">
+        <v>111</v>
+      </c>
+      <c r="B307" s="146">
+        <v>0.94969999999999999</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A308" s="145" t="s">
+        <v>112</v>
+      </c>
+      <c r="B308" s="146">
+        <v>0.98499999999999999</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A309" s="145" t="s">
         <v>531</v>
       </c>
-      <c r="B307" s="146">
+      <c r="B309" s="146">
         <v>0.7</v>
-      </c>
-    </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A308" s="147" t="s">
-        <v>505</v>
-      </c>
-      <c r="B308" s="148" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A309" s="147" t="s">
-        <v>507</v>
-      </c>
-      <c r="B309" s="148" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A310" s="147" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B310" s="148" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A311" s="147" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="B311" s="148" t="s">
-        <v>77</v>
+        <v>508</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A312" s="147" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="B312" s="148" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A313" s="147" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="B313" s="148" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A314" s="147" t="s">
+        <v>512</v>
+      </c>
+      <c r="B314" s="148" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A315" s="147" t="s">
+        <v>514</v>
+      </c>
+      <c r="B315" s="148" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A316" s="147" t="s">
         <v>515</v>
       </c>
-      <c r="B314" s="148" t="s">
+      <c r="B316" s="148" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A315" s="145" t="s">
-        <v>544</v>
-      </c>
-      <c r="B315" s="146"/>
-    </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A316" s="145" t="s">
-        <v>517</v>
-      </c>
-      <c r="B316" s="146"/>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A317" s="145" t="s">
-        <v>694</v>
+        <v>544</v>
       </c>
       <c r="B317" s="146"/>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A318" s="145" t="s">
-        <v>695</v>
+        <v>517</v>
       </c>
       <c r="B318" s="146"/>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A319" s="145" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="B319" s="146"/>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A320" s="145" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="B320" s="146"/>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A321" s="145" t="s">
+        <v>696</v>
+      </c>
+      <c r="B321" s="146"/>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A322" s="145" t="s">
+        <v>697</v>
+      </c>
+      <c r="B322" s="146"/>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A323" s="145" t="s">
         <v>564</v>
       </c>
-      <c r="B321" s="146"/>
+      <c r="B323" s="146"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11436,10 +12471,861 @@
   <sheetPr>
     <tabColor rgb="FF15FFC2"/>
   </sheetPr>
+  <dimension ref="A1:R16"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="13.3125" style="191" customWidth="1"/>
+    <col min="2" max="2" width="3.3671875" style="191" customWidth="1"/>
+    <col min="3" max="3" width="11.3671875" style="191" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.05078125" style="191" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="3.68359375" style="191" customWidth="1"/>
+    <col min="9" max="9" width="4.3671875" style="191" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.1015625" style="191" customWidth="1"/>
+    <col min="11" max="14" width="4.3671875" style="191" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.20703125" style="191" customWidth="1"/>
+    <col min="16" max="16" width="4.3671875" style="191" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.68359375" style="191" customWidth="1"/>
+    <col min="18" max="18" width="54.7890625" style="191" customWidth="1"/>
+    <col min="19" max="16384" width="8.83984375" style="191"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="188"/>
+      <c r="B1" s="189"/>
+      <c r="C1" s="186" t="s">
+        <v>602</v>
+      </c>
+      <c r="D1" s="187" t="s">
+        <v>581</v>
+      </c>
+      <c r="E1" s="197" t="s">
+        <v>589</v>
+      </c>
+      <c r="F1" s="198" t="s">
+        <v>590</v>
+      </c>
+      <c r="G1" s="198" t="s">
+        <v>591</v>
+      </c>
+      <c r="H1" s="199" t="s">
+        <v>592</v>
+      </c>
+      <c r="I1" s="200" t="s">
+        <v>593</v>
+      </c>
+      <c r="J1" s="201" t="s">
+        <v>594</v>
+      </c>
+      <c r="K1" s="201" t="s">
+        <v>595</v>
+      </c>
+      <c r="L1" s="202" t="s">
+        <v>596</v>
+      </c>
+      <c r="M1" s="203" t="s">
+        <v>597</v>
+      </c>
+      <c r="N1" s="204" t="s">
+        <v>598</v>
+      </c>
+      <c r="O1" s="204" t="s">
+        <v>599</v>
+      </c>
+      <c r="P1" s="205" t="s">
+        <v>600</v>
+      </c>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="190" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A2" s="192"/>
+      <c r="B2" s="193">
+        <v>0</v>
+      </c>
+      <c r="C2" s="206" t="s">
+        <v>586</v>
+      </c>
+      <c r="D2" s="207">
+        <v>1</v>
+      </c>
+      <c r="E2" s="208">
+        <v>1</v>
+      </c>
+      <c r="F2" s="209">
+        <v>3</v>
+      </c>
+      <c r="G2" s="209">
+        <v>9</v>
+      </c>
+      <c r="H2" s="210">
+        <v>11</v>
+      </c>
+      <c r="I2" s="211">
+        <v>0.4</v>
+      </c>
+      <c r="J2" s="212">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="212">
+        <v>1.25</v>
+      </c>
+      <c r="L2" s="213">
+        <v>0.75</v>
+      </c>
+      <c r="M2" s="214">
+        <v>0.75</v>
+      </c>
+      <c r="N2" s="215">
+        <v>0.75</v>
+      </c>
+      <c r="O2" s="215">
+        <v>0.5</v>
+      </c>
+      <c r="P2" s="216">
+        <v>0.1</v>
+      </c>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="194" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A3" s="192"/>
+      <c r="B3" s="193">
+        <v>1</v>
+      </c>
+      <c r="C3" s="206" t="s">
+        <v>610</v>
+      </c>
+      <c r="D3" s="207">
+        <v>6</v>
+      </c>
+      <c r="E3" s="217">
+        <v>2</v>
+      </c>
+      <c r="F3" s="218">
+        <v>5</v>
+      </c>
+      <c r="G3" s="218">
+        <v>14</v>
+      </c>
+      <c r="H3" s="219">
+        <v>17</v>
+      </c>
+      <c r="I3" s="220">
+        <v>0.4</v>
+      </c>
+      <c r="J3" s="221">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="221">
+        <v>1.25</v>
+      </c>
+      <c r="L3" s="222">
+        <v>0.75</v>
+      </c>
+      <c r="M3" s="223">
+        <v>0.75</v>
+      </c>
+      <c r="N3" s="224">
+        <v>0.75</v>
+      </c>
+      <c r="O3" s="224">
+        <v>0.5</v>
+      </c>
+      <c r="P3" s="225">
+        <v>0.1</v>
+      </c>
+      <c r="Q3" s="51"/>
+      <c r="R3" s="195" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A4" s="192"/>
+      <c r="B4" s="193">
+        <v>2</v>
+      </c>
+      <c r="C4" s="206" t="s">
+        <v>611</v>
+      </c>
+      <c r="D4" s="207">
+        <v>11</v>
+      </c>
+      <c r="E4" s="217">
+        <v>1</v>
+      </c>
+      <c r="F4" s="218">
+        <v>4</v>
+      </c>
+      <c r="G4" s="218">
+        <v>12</v>
+      </c>
+      <c r="H4" s="219">
+        <v>15</v>
+      </c>
+      <c r="I4" s="220">
+        <v>0.4</v>
+      </c>
+      <c r="J4" s="221">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="221">
+        <v>1.25</v>
+      </c>
+      <c r="L4" s="222">
+        <v>0.75</v>
+      </c>
+      <c r="M4" s="223">
+        <v>0.75</v>
+      </c>
+      <c r="N4" s="224">
+        <v>0.75</v>
+      </c>
+      <c r="O4" s="224">
+        <v>0.5</v>
+      </c>
+      <c r="P4" s="225">
+        <v>0.1</v>
+      </c>
+      <c r="Q4" s="51"/>
+      <c r="R4" s="195" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A5" s="192"/>
+      <c r="B5" s="193">
+        <v>3</v>
+      </c>
+      <c r="C5" s="206" t="s">
+        <v>612</v>
+      </c>
+      <c r="D5" s="207">
+        <v>1</v>
+      </c>
+      <c r="E5" s="217">
+        <v>1</v>
+      </c>
+      <c r="F5" s="218">
+        <v>3</v>
+      </c>
+      <c r="G5" s="218">
+        <v>10</v>
+      </c>
+      <c r="H5" s="219">
+        <v>12</v>
+      </c>
+      <c r="I5" s="220">
+        <v>0.4</v>
+      </c>
+      <c r="J5" s="221">
+        <v>0.8</v>
+      </c>
+      <c r="K5" s="221">
+        <v>1.25</v>
+      </c>
+      <c r="L5" s="222">
+        <v>0.75</v>
+      </c>
+      <c r="M5" s="223">
+        <v>0.75</v>
+      </c>
+      <c r="N5" s="224">
+        <v>0.75</v>
+      </c>
+      <c r="O5" s="224">
+        <v>0.5</v>
+      </c>
+      <c r="P5" s="225">
+        <v>0.1</v>
+      </c>
+      <c r="Q5" s="51"/>
+      <c r="R5" s="195" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A6" s="192"/>
+      <c r="B6" s="193">
+        <v>4</v>
+      </c>
+      <c r="C6" s="206" t="s">
+        <v>585</v>
+      </c>
+      <c r="D6" s="207">
+        <v>11</v>
+      </c>
+      <c r="E6" s="217">
+        <v>1</v>
+      </c>
+      <c r="F6" s="218">
+        <v>2</v>
+      </c>
+      <c r="G6" s="218">
+        <v>4</v>
+      </c>
+      <c r="H6" s="219">
+        <v>5</v>
+      </c>
+      <c r="I6" s="220">
+        <v>0.4</v>
+      </c>
+      <c r="J6" s="221">
+        <v>0.75</v>
+      </c>
+      <c r="K6" s="221">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="L6" s="222">
+        <v>0.4</v>
+      </c>
+      <c r="M6" s="223">
+        <v>0.2</v>
+      </c>
+      <c r="N6" s="224">
+        <v>0.65</v>
+      </c>
+      <c r="O6" s="224">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P6" s="225">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="Q6" s="51"/>
+      <c r="R6" s="195"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A7" s="192"/>
+      <c r="B7" s="193">
+        <v>5</v>
+      </c>
+      <c r="C7" s="206" t="s">
+        <v>729</v>
+      </c>
+      <c r="D7" s="207">
+        <v>6</v>
+      </c>
+      <c r="E7" s="217">
+        <v>1</v>
+      </c>
+      <c r="F7" s="218">
+        <v>2</v>
+      </c>
+      <c r="G7" s="218">
+        <v>4</v>
+      </c>
+      <c r="H7" s="219">
+        <v>5</v>
+      </c>
+      <c r="I7" s="226">
+        <v>0.6</v>
+      </c>
+      <c r="J7" s="227">
+        <v>0.9</v>
+      </c>
+      <c r="K7" s="227">
+        <v>1.2</v>
+      </c>
+      <c r="L7" s="228">
+        <v>0.8</v>
+      </c>
+      <c r="M7" s="229">
+        <v>0.4</v>
+      </c>
+      <c r="N7" s="230">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O7" s="230">
+        <v>0.8</v>
+      </c>
+      <c r="P7" s="231">
+        <v>0.4</v>
+      </c>
+      <c r="Q7" s="51"/>
+      <c r="R7" s="195" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A8" s="192"/>
+      <c r="B8" s="193">
+        <v>6</v>
+      </c>
+      <c r="C8" s="206" t="s">
+        <v>730</v>
+      </c>
+      <c r="D8" s="207">
+        <v>11</v>
+      </c>
+      <c r="E8" s="217">
+        <v>1</v>
+      </c>
+      <c r="F8" s="218">
+        <v>2</v>
+      </c>
+      <c r="G8" s="218">
+        <v>4</v>
+      </c>
+      <c r="H8" s="219">
+        <v>5</v>
+      </c>
+      <c r="I8" s="226">
+        <v>0.7</v>
+      </c>
+      <c r="J8" s="227">
+        <v>0.9</v>
+      </c>
+      <c r="K8" s="227">
+        <v>1.05</v>
+      </c>
+      <c r="L8" s="228">
+        <v>0.75</v>
+      </c>
+      <c r="M8" s="229">
+        <v>0.45</v>
+      </c>
+      <c r="N8" s="230">
+        <v>0.65</v>
+      </c>
+      <c r="O8" s="230">
+        <v>0.8</v>
+      </c>
+      <c r="P8" s="231">
+        <v>0.3</v>
+      </c>
+      <c r="Q8" s="51"/>
+      <c r="R8" s="195" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A9" s="192"/>
+      <c r="B9" s="193">
+        <v>7</v>
+      </c>
+      <c r="C9" s="206" t="s">
+        <v>731</v>
+      </c>
+      <c r="D9" s="207">
+        <v>6</v>
+      </c>
+      <c r="E9" s="217">
+        <v>1</v>
+      </c>
+      <c r="F9" s="218">
+        <v>2</v>
+      </c>
+      <c r="G9" s="218">
+        <v>4</v>
+      </c>
+      <c r="H9" s="219">
+        <v>5</v>
+      </c>
+      <c r="I9" s="220">
+        <v>0.3</v>
+      </c>
+      <c r="J9" s="221">
+        <v>0.75</v>
+      </c>
+      <c r="K9" s="221">
+        <v>1.2</v>
+      </c>
+      <c r="L9" s="222">
+        <v>0.5</v>
+      </c>
+      <c r="M9" s="223">
+        <v>0.4</v>
+      </c>
+      <c r="N9" s="224">
+        <v>0.4</v>
+      </c>
+      <c r="O9" s="224">
+        <v>1.3</v>
+      </c>
+      <c r="P9" s="225">
+        <v>0.5</v>
+      </c>
+      <c r="Q9" s="51"/>
+      <c r="R9" s="195" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A10" s="196"/>
+      <c r="B10" s="193">
+        <v>8</v>
+      </c>
+      <c r="C10" s="206" t="s">
+        <v>732</v>
+      </c>
+      <c r="D10" s="207">
+        <v>11</v>
+      </c>
+      <c r="E10" s="217">
+        <v>1</v>
+      </c>
+      <c r="F10" s="218">
+        <v>2</v>
+      </c>
+      <c r="G10" s="218">
+        <v>4</v>
+      </c>
+      <c r="H10" s="219">
+        <v>5</v>
+      </c>
+      <c r="I10" s="220">
+        <v>0.3</v>
+      </c>
+      <c r="J10" s="221">
+        <v>0.75</v>
+      </c>
+      <c r="K10" s="221">
+        <v>1.2</v>
+      </c>
+      <c r="L10" s="222">
+        <v>0.5</v>
+      </c>
+      <c r="M10" s="223">
+        <v>0.4</v>
+      </c>
+      <c r="N10" s="224">
+        <v>0.4</v>
+      </c>
+      <c r="O10" s="224">
+        <v>1.3</v>
+      </c>
+      <c r="P10" s="225">
+        <v>0.5</v>
+      </c>
+      <c r="Q10" s="51"/>
+      <c r="R10" s="195" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A11" s="196"/>
+      <c r="B11" s="193">
+        <v>9</v>
+      </c>
+      <c r="C11" s="206" t="s">
+        <v>725</v>
+      </c>
+      <c r="D11" s="207">
+        <v>4</v>
+      </c>
+      <c r="E11" s="217">
+        <v>1</v>
+      </c>
+      <c r="F11" s="218">
+        <v>2</v>
+      </c>
+      <c r="G11" s="218">
+        <v>5</v>
+      </c>
+      <c r="H11" s="219">
+        <v>7</v>
+      </c>
+      <c r="I11" s="226">
+        <v>0.46</v>
+      </c>
+      <c r="J11" s="227">
+        <v>0.7</v>
+      </c>
+      <c r="K11" s="227">
+        <v>1.01</v>
+      </c>
+      <c r="L11" s="228">
+        <v>0.39</v>
+      </c>
+      <c r="M11" s="229">
+        <v>0.2</v>
+      </c>
+      <c r="N11" s="230">
+        <v>0.5</v>
+      </c>
+      <c r="O11" s="230">
+        <v>0.5</v>
+      </c>
+      <c r="P11" s="231">
+        <v>0.25</v>
+      </c>
+      <c r="R11" s="195"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A12" s="196"/>
+      <c r="B12" s="193">
+        <v>10</v>
+      </c>
+      <c r="C12" s="206" t="s">
+        <v>727</v>
+      </c>
+      <c r="D12" s="207">
+        <v>6</v>
+      </c>
+      <c r="E12" s="217">
+        <v>1</v>
+      </c>
+      <c r="F12" s="218">
+        <v>2</v>
+      </c>
+      <c r="G12" s="218">
+        <v>4</v>
+      </c>
+      <c r="H12" s="219">
+        <v>5</v>
+      </c>
+      <c r="I12" s="226">
+        <v>0.5</v>
+      </c>
+      <c r="J12" s="227">
+        <v>0.8</v>
+      </c>
+      <c r="K12" s="227">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="L12" s="228">
+        <v>0.5</v>
+      </c>
+      <c r="M12" s="229">
+        <v>0.2</v>
+      </c>
+      <c r="N12" s="230">
+        <v>0.8</v>
+      </c>
+      <c r="O12" s="230">
+        <v>0.8</v>
+      </c>
+      <c r="P12" s="231">
+        <v>1</v>
+      </c>
+      <c r="R12" s="195"/>
+    </row>
+    <row r="13" spans="1:18" ht="13.2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="196"/>
+      <c r="B13" s="193">
+        <v>11</v>
+      </c>
+      <c r="C13" s="206" t="s">
+        <v>728</v>
+      </c>
+      <c r="D13" s="207">
+        <v>11</v>
+      </c>
+      <c r="E13" s="217">
+        <v>1</v>
+      </c>
+      <c r="F13" s="218">
+        <v>2</v>
+      </c>
+      <c r="G13" s="218">
+        <v>4</v>
+      </c>
+      <c r="H13" s="219">
+        <v>5</v>
+      </c>
+      <c r="I13" s="220">
+        <v>0.4</v>
+      </c>
+      <c r="J13" s="221">
+        <v>0.75</v>
+      </c>
+      <c r="K13" s="221">
+        <v>1.05</v>
+      </c>
+      <c r="L13" s="222">
+        <v>0.35</v>
+      </c>
+      <c r="M13" s="223">
+        <v>0.2</v>
+      </c>
+      <c r="N13" s="224">
+        <v>0.8</v>
+      </c>
+      <c r="O13" s="224">
+        <v>0.6</v>
+      </c>
+      <c r="P13" s="225">
+        <v>0.2</v>
+      </c>
+      <c r="R13" s="195"/>
+    </row>
+    <row r="14" spans="1:18" ht="13.2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="196"/>
+      <c r="B14" s="193">
+        <v>12</v>
+      </c>
+      <c r="C14" s="206" t="s">
+        <v>584</v>
+      </c>
+      <c r="D14" s="207">
+        <v>6</v>
+      </c>
+      <c r="E14" s="217">
+        <v>1</v>
+      </c>
+      <c r="F14" s="218">
+        <v>2</v>
+      </c>
+      <c r="G14" s="218">
+        <v>4</v>
+      </c>
+      <c r="H14" s="219">
+        <v>5</v>
+      </c>
+      <c r="I14" s="220">
+        <v>0.4</v>
+      </c>
+      <c r="J14" s="221">
+        <v>0.75</v>
+      </c>
+      <c r="K14" s="221">
+        <v>1.05</v>
+      </c>
+      <c r="L14" s="222">
+        <v>0.6</v>
+      </c>
+      <c r="M14" s="223">
+        <v>0.2</v>
+      </c>
+      <c r="N14" s="224">
+        <v>0.8</v>
+      </c>
+      <c r="O14" s="224">
+        <v>0.6</v>
+      </c>
+      <c r="P14" s="225">
+        <v>0.2</v>
+      </c>
+      <c r="R14" s="232" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="13.2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="196"/>
+      <c r="B15" s="193">
+        <v>13</v>
+      </c>
+      <c r="C15" s="206" t="s">
+        <v>583</v>
+      </c>
+      <c r="D15" s="207">
+        <v>11</v>
+      </c>
+      <c r="E15" s="217">
+        <v>1</v>
+      </c>
+      <c r="F15" s="218">
+        <v>2</v>
+      </c>
+      <c r="G15" s="218">
+        <v>3</v>
+      </c>
+      <c r="H15" s="219">
+        <v>4</v>
+      </c>
+      <c r="I15" s="220">
+        <v>0.42</v>
+      </c>
+      <c r="J15" s="221">
+        <v>0.71</v>
+      </c>
+      <c r="K15" s="221">
+        <v>0.62</v>
+      </c>
+      <c r="L15" s="222">
+        <v>0.23</v>
+      </c>
+      <c r="M15" s="223">
+        <v>0.2</v>
+      </c>
+      <c r="N15" s="224">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="O15" s="224">
+        <v>0.45</v>
+      </c>
+      <c r="P15" s="225">
+        <v>0.2</v>
+      </c>
+      <c r="R15" s="233" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="13.2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="196"/>
+      <c r="B16" s="193">
+        <v>14</v>
+      </c>
+      <c r="C16" s="206" t="s">
+        <v>588</v>
+      </c>
+      <c r="D16" s="207">
+        <v>11</v>
+      </c>
+      <c r="E16" s="217">
+        <v>1</v>
+      </c>
+      <c r="F16" s="218">
+        <v>2</v>
+      </c>
+      <c r="G16" s="218">
+        <v>4</v>
+      </c>
+      <c r="H16" s="219">
+        <v>5</v>
+      </c>
+      <c r="I16" s="220">
+        <v>0.3</v>
+      </c>
+      <c r="J16" s="221">
+        <v>0.75</v>
+      </c>
+      <c r="K16" s="221">
+        <v>1.2</v>
+      </c>
+      <c r="L16" s="222">
+        <v>0.5</v>
+      </c>
+      <c r="M16" s="223">
+        <v>0.4</v>
+      </c>
+      <c r="N16" s="224">
+        <v>0.4</v>
+      </c>
+      <c r="O16" s="224">
+        <v>1.3</v>
+      </c>
+      <c r="P16" s="225">
+        <v>0.5</v>
+      </c>
+      <c r="R16" s="234" t="s">
+        <v>752</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C2D2EFD-B359-4BA7-8894-C1EBC96E92BC}">
+  <sheetPr>
+    <tabColor rgb="FF15FFC2"/>
+  </sheetPr>
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -11914,7 +13800,28 @@
       <c r="R9" s="72"/>
     </row>
     <row r="10" spans="1:18" ht="12.9" x14ac:dyDescent="0.5">
+      <c r="C10" s="49" t="s">
+        <v>725</v>
+      </c>
+      <c r="D10" s="49">
+        <v>4</v>
+      </c>
+      <c r="E10" s="49">
+        <v>1</v>
+      </c>
+      <c r="F10" s="49">
+        <v>2</v>
+      </c>
+      <c r="G10" s="49">
+        <v>5</v>
+      </c>
+      <c r="H10" s="49">
+        <v>7</v>
+      </c>
       <c r="Q10" s="51"/>
+      <c r="R10" s="49" t="s">
+        <v>726</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11923,136 +13830,180 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13DE2398-4D66-4F9C-BA4E-2DE4F9D6B687}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="B1:D8"/>
+      <selection activeCell="B4" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
+    <col min="1" max="1" width="20.578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.05078125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.1015625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="109"/>
-      <c r="B1" s="74" t="s">
-        <v>602</v>
-      </c>
-      <c r="C1" s="74" t="s">
-        <v>581</v>
-      </c>
-      <c r="D1" s="77" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="110">
-        <v>1</v>
-      </c>
-      <c r="B2" s="54" t="s">
-        <v>610</v>
-      </c>
-      <c r="C2" s="59">
-        <v>7</v>
-      </c>
-      <c r="D2" s="62">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="110">
-        <v>2</v>
-      </c>
-      <c r="B3" s="63" t="s">
-        <v>611</v>
-      </c>
-      <c r="C3" s="59">
-        <v>10</v>
-      </c>
-      <c r="D3" s="62">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="110">
-        <v>3</v>
-      </c>
-      <c r="B4" s="63" t="s">
-        <v>612</v>
-      </c>
-      <c r="C4" s="59">
-        <v>1</v>
-      </c>
-      <c r="D4" s="62">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="110">
-        <v>4</v>
-      </c>
-      <c r="B5" s="63" t="s">
-        <v>583</v>
-      </c>
-      <c r="C5" s="59">
-        <v>11</v>
-      </c>
-      <c r="D5" s="62">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="110">
-        <v>5</v>
-      </c>
-      <c r="B6" s="63" t="s">
-        <v>584</v>
-      </c>
-      <c r="C6" s="59">
-        <v>6</v>
-      </c>
-      <c r="D6" s="62">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="110">
-        <v>6</v>
-      </c>
-      <c r="B7" s="63" t="s">
-        <v>585</v>
-      </c>
-      <c r="C7" s="59">
-        <v>11</v>
-      </c>
-      <c r="D7" s="62">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="110">
-        <v>7</v>
-      </c>
-      <c r="B8" s="63" t="s">
-        <v>588</v>
-      </c>
-      <c r="C8" s="59">
-        <v>11</v>
-      </c>
-      <c r="D8" s="62">
-        <v>5</v>
-      </c>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>755</v>
+      </c>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="237"/>
+      <c r="F1" s="237"/>
+      <c r="G1" s="237"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="238"/>
+      <c r="C2" s="238"/>
+      <c r="D2" s="238"/>
+      <c r="E2" s="237"/>
+      <c r="F2" s="237"/>
+      <c r="G2" s="237"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="104" t="s">
+        <v>517</v>
+      </c>
+      <c r="B3" s="235" t="s">
+        <v>754</v>
+      </c>
+      <c r="C3" s="238"/>
+      <c r="D3" s="238"/>
+      <c r="E3" s="237"/>
+      <c r="F3" s="237"/>
+      <c r="G3" s="237"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="104" t="s">
+        <v>561</v>
+      </c>
+      <c r="B4" s="170" t="s">
+        <v>707</v>
+      </c>
+      <c r="C4" s="238"/>
+      <c r="D4" s="238"/>
+      <c r="E4" s="237"/>
+      <c r="F4" s="237"/>
+      <c r="G4" s="237"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="145" t="s">
+        <v>695</v>
+      </c>
+      <c r="B5" s="170" t="s">
+        <v>709</v>
+      </c>
+      <c r="C5" s="238"/>
+      <c r="D5" s="238"/>
+      <c r="E5" s="237"/>
+      <c r="F5" s="237"/>
+      <c r="G5" s="237"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="235"/>
+      <c r="B6" s="238"/>
+      <c r="C6" s="238"/>
+      <c r="D6" s="238"/>
+      <c r="E6" s="237"/>
+      <c r="F6" s="237"/>
+      <c r="G6" s="237"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="235"/>
+      <c r="B7" s="238"/>
+      <c r="C7" s="238"/>
+      <c r="D7" s="238"/>
+      <c r="E7" s="237"/>
+      <c r="F7" s="237"/>
+      <c r="G7" s="237"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="235"/>
+      <c r="B8" s="238"/>
+      <c r="C8" s="238"/>
+      <c r="D8" s="238"/>
+      <c r="E8" s="237"/>
+      <c r="F8" s="237"/>
+      <c r="G8" s="237"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="237"/>
+      <c r="B9" s="237"/>
+      <c r="C9" s="237"/>
+      <c r="D9" s="237"/>
+      <c r="E9" s="237"/>
+      <c r="F9" s="237"/>
+      <c r="G9" s="237"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="237"/>
+      <c r="B10" s="237"/>
+      <c r="C10" s="237"/>
+      <c r="D10" s="237"/>
+      <c r="E10" s="237"/>
+      <c r="F10" s="237"/>
+      <c r="G10" s="237"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="237"/>
+      <c r="B11" s="237"/>
+      <c r="C11" s="237"/>
+      <c r="D11" s="237"/>
+      <c r="E11" s="237"/>
+      <c r="F11" s="237"/>
+      <c r="G11" s="237"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="237"/>
+      <c r="B12" s="237"/>
+      <c r="C12" s="237"/>
+      <c r="D12" s="237"/>
+      <c r="E12" s="237"/>
+      <c r="F12" s="237"/>
+      <c r="G12" s="237"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="237"/>
+      <c r="B13" s="237"/>
+      <c r="C13" s="237"/>
+      <c r="D13" s="237"/>
+      <c r="E13" s="237"/>
+      <c r="F13" s="237"/>
+      <c r="G13" s="237"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="237"/>
+      <c r="B14" s="237"/>
+      <c r="C14" s="237"/>
+      <c r="D14" s="237"/>
+      <c r="E14" s="237"/>
+      <c r="F14" s="237"/>
+      <c r="G14" s="237"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="237"/>
+      <c r="B15" s="237"/>
+      <c r="C15" s="237"/>
+      <c r="D15" s="237"/>
+      <c r="E15" s="237"/>
+      <c r="F15" s="237"/>
+      <c r="G15" s="237"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B4:B5">
+    <cfRule type="notContainsErrors" dxfId="6" priority="2">
+      <formula>NOT(ISERROR(B4))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A0B17ED-365F-42A2-8A56-1051B9FEC7F3}">
   <dimension ref="A1:E46"/>
   <sheetViews>
@@ -12486,7 +14437,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F68B577-1ED3-4341-9ED6-7148A85D6559}">
   <dimension ref="A1:G503"/>
   <sheetViews>
@@ -16492,466 +18443,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811BB740-2696-4061-9D1F-96ECA011A915}">
-  <dimension ref="A1:G40"/>
-  <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="1" width="21.3125" style="21" customWidth="1"/>
-    <col min="2" max="2" width="25.62890625" style="23" customWidth="1"/>
-    <col min="3" max="3" width="1.734375" style="23" customWidth="1"/>
-    <col min="4" max="4" width="73" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83984375" style="21"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="A1" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="41" t="s">
-        <v>123</v>
-      </c>
-      <c r="B2" s="42" t="s">
-        <v>578</v>
-      </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="42" t="s">
-        <v>577</v>
-      </c>
-      <c r="E2" s="32"/>
-    </row>
-    <row r="3" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A3" s="41" t="s">
-        <v>124</v>
-      </c>
-      <c r="B3" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="41" t="s">
-        <v>126</v>
-      </c>
-      <c r="B4" s="42">
-        <v>10</v>
-      </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="33" t="s">
-        <v>566</v>
-      </c>
-      <c r="E4" s="32"/>
-      <c r="F4" s="22" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="41" t="s">
-        <v>407</v>
-      </c>
-      <c r="B5" s="42">
-        <v>1</v>
-      </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="41" t="s">
-        <v>557</v>
-      </c>
-      <c r="B6" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="41" t="s">
-        <v>544</v>
-      </c>
-      <c r="B7" s="42" t="s">
-        <v>582</v>
-      </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="32"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="41" t="s">
-        <v>517</v>
-      </c>
-      <c r="B8" s="48" t="s">
-        <v>571</v>
-      </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="41" t="s">
-        <v>561</v>
-      </c>
-      <c r="B9" s="42"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="41" t="s">
-        <v>562</v>
-      </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="41" t="s">
-        <v>563</v>
-      </c>
-      <c r="B11" s="42"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="41" t="s">
-        <v>564</v>
-      </c>
-      <c r="B12" s="43" t="s">
-        <v>565</v>
-      </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="41" t="s">
-        <v>100</v>
-      </c>
-      <c r="B13" s="42" t="s">
-        <v>532</v>
-      </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="B14" s="42" t="s">
-        <v>533</v>
-      </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="41" t="s">
-        <v>103</v>
-      </c>
-      <c r="B15" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="41" t="s">
-        <v>117</v>
-      </c>
-      <c r="B16" s="42" t="s">
-        <v>560</v>
-      </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" s="42" t="b">
-        <v>0</v>
-      </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="41" t="s">
-        <v>105</v>
-      </c>
-      <c r="B18" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="41" t="s">
-        <v>127</v>
-      </c>
-      <c r="B19" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="41" t="s">
-        <v>128</v>
-      </c>
-      <c r="B20" s="42" t="s">
-        <v>568</v>
-      </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="35" t="s">
-        <v>558</v>
-      </c>
-      <c r="E20" s="32"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="B21" s="42" t="b">
-        <v>0</v>
-      </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-    </row>
-    <row r="22" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A22" s="41" t="s">
-        <v>130</v>
-      </c>
-      <c r="B22" s="42" t="s">
-        <v>559</v>
-      </c>
-      <c r="C22" s="26"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="B23" s="33" t="s">
-        <v>567</v>
-      </c>
-      <c r="C23" s="26"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="44" t="s">
-        <v>390</v>
-      </c>
-      <c r="B24" s="42" t="b">
-        <v>0</v>
-      </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="44" t="s">
-        <v>391</v>
-      </c>
-      <c r="B25" s="42" t="b">
-        <v>0</v>
-      </c>
-      <c r="C25" s="29"/>
-      <c r="D25" s="32" t="s">
-        <v>572</v>
-      </c>
-      <c r="E25" s="32" t="s">
-        <v>573</v>
-      </c>
-      <c r="F25" s="21" t="s">
-        <v>574</v>
-      </c>
-      <c r="G25" s="21" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="B26" s="45">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="36">
-        <v>8.0484411999999994E-6</v>
-      </c>
-      <c r="E26" s="36">
-        <v>3.0484411999999999E-6</v>
-      </c>
-      <c r="F26" s="24">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="G26" s="24">
-        <v>2.0000000000000002E-5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="44" t="s">
-        <v>551</v>
-      </c>
-      <c r="B27" s="46">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="C27" s="31"/>
-      <c r="D27" s="32">
-        <v>0.01</v>
-      </c>
-      <c r="E27" s="37">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="F27" s="21">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="G27" s="21">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="44" t="s">
-        <v>171</v>
-      </c>
-      <c r="B28" s="42" t="s">
-        <v>569</v>
-      </c>
-      <c r="C28" s="29"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="44" t="s">
-        <v>173</v>
-      </c>
-      <c r="B29" s="42" t="s">
-        <v>570</v>
-      </c>
-      <c r="C29" s="29"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>278</v>
-      </c>
-      <c r="C30" s="29"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="C31" s="29"/>
-      <c r="E31" s="32"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="C32" s="29"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="47"/>
-      <c r="B33" s="42"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="47"/>
-      <c r="B34" s="42"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="47"/>
-      <c r="B35" s="42"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="47"/>
-      <c r="B36" s="42"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="47"/>
-      <c r="B37" s="42"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="47"/>
-      <c r="B38" s="42"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="47"/>
-      <c r="B39" s="42"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="47"/>
-      <c r="B40" s="42"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Developments, updates, and improvements
</commit_message>
<xml_diff>
--- a/CWatM_settings/cwatm_settings.xlsx
+++ b/CWatM_settings/cwatm_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\FUSE\CWatM_settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1591BB3-E8F6-46B0-9472-3E80079258D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEA064A-BB07-44F9-BFAD-0806E98ED563}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="852" yWindow="-96" windowWidth="22284" windowHeight="13152" tabRatio="820" xr2:uid="{3B47940C-5F20-42D1-80D0-733DA86DBAA8}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="229">
   <si>
     <t>Key</t>
   </si>
@@ -718,21 +718,6 @@
     <t>actual_totalWithdrawal, precipEffectiveAverage_segments, precipEffectiveAverage_woBare_segments</t>
   </si>
   <si>
-    <t>$(PathLandcover)/fracVegCover[0]_monthend.nc</t>
-  </si>
-  <si>
-    <t>$(PathLandcover)/fracVegCover[4]_monthend.nc</t>
-  </si>
-  <si>
-    <t>$(PathLandcover)/fracVegCover[3]_monthend.nc</t>
-  </si>
-  <si>
-    <t>$(PathLandcover)/fracVegCover[2]_monthend.nc</t>
-  </si>
-  <si>
-    <t>$(PathLandcover)/fracVegCover[5]_monthend.nc</t>
-  </si>
-  <si>
     <t>[1, ~7]</t>
   </si>
   <si>
@@ -745,61 +730,52 @@
     <t>Chickpea adapted</t>
   </si>
   <si>
-    <t>Forest_fraction</t>
-  </si>
-  <si>
-    <t>Sealed_fraction</t>
-  </si>
-  <si>
-    <t>IrrigationEquipped_fraction</t>
-  </si>
-  <si>
-    <t>Water_fraction</t>
-  </si>
-  <si>
-    <t>Paddy_fraction</t>
-  </si>
-  <si>
     <t>activate_fallow</t>
   </si>
   <si>
     <t>010deg</t>
   </si>
   <si>
+    <t>$(FILE_PATHS:PathMaps)/init/Bhima_20160501.nc</t>
+  </si>
+  <si>
+    <t>$(FILE_PATHS:PathMaps)/init/Bhima_20150505.nc</t>
+  </si>
+  <si>
+    <t>act_irrWithdrawalSW, act_irrWithdrawalGW, act_nonIrrWithdrawalSW, act_nonIrrWithdrawalGW, actual_totalWithdrawal, actTransTotal_grasslands, actTransTotal_nonpaddy, discharge, act_irrWithdrawal, act_nonIrrWithdrawal</t>
+  </si>
+  <si>
+    <t>automaticFallowingIrr</t>
+  </si>
+  <si>
+    <t>True for MS, False for FUSE</t>
+  </si>
+  <si>
+    <t>waterBodyID, resVolume_reservoir, cellArea, adminSegments, GeneralCrop_Irr, modflowtotalSoilThickness, adminSegments, reservoir_command_areas, lift_command_areas</t>
+  </si>
+  <si>
+    <t>reservoir_command_areas</t>
+  </si>
+  <si>
+    <t>$(PathWaterdemand)/CommandLiftAreas_15Oct.tif</t>
+  </si>
+  <si>
     <t>head_development_segments, modflowWaterLevel, fracVegCover[0], fracVegCover[1], fracVegCover[2], fracVegCover[3], fracVegCover[4], fracVegCover[5], frac_totalIrr, frac_totalnonIrr, fracCrops_Irr[0],  fracCrops_Irr[1], fracCrops_Irr[2], fracCrops_Irr[3], fracCrops_Irr[4], fracCrops_Irr[5], fracCrops_Irr[6], fracCrops_Irr[7], fracCrops_Irr[8], fracCrops_Irr[9], fracCrops_Irr[10], fracCrops_Irr[11], fracCrops_Irr[12], fracCrops_Irr[13], fracCrops_Irr[14], fracCrops_Irr[15], fracCrops_Irr[16], fracCrops_Irr[17], fracCrops_nonIrr[0], fracCrops_nonIrr[1], fracCrops_nonIrr[2], fracCrops_nonIrr[3], fracCrops_nonIrr[4], fracCrops_nonIrr[5], fracCrops_nonIrr[6], fracCrops_nonIrr[7],  fracCrops_nonIrr[8], fracCrops_nonIrr[9], fracCrops_nonIrr[10], fracCrops_nonIrr[11], fracCrops_nonIrr[12], fracCrops_nonIrr[13], fracCrops_nonIrr[14], fracCrops_nonIrr[15], fracCrops_nonIrr[16], fracCrops_nonIrr[17], fracCrops_IrrLandDemand[0],  fracCrops_IrrLandDemand[1], fracCrops_IrrLandDemand[2], fracCrops_IrrLandDemand[3], fracCrops_IrrLandDemand[4], fracCrops_IrrLandDemand[5], fracCrops_IrrLandDemand[6], fracCrops_IrrLandDemand[7],fracCrops_IrrLandDemand[8], fracCrops_IrrLandDemand[9], fracCrops_IrrLandDemand[10], fracCrops_IrrLandDemand[11], fracCrops_IrrLandDemand[12], fracCrops_IrrLandDemand[13], fracCrops_IrrLandDemand[14], fracCrops_IrrLandDemand[15], fracCrops_IrrLandDemand[16], fracCrops_IrrLandDemand[17], fracCrops_nonIrrLandDemand[0],  fracCrops_nonIrrLandDemand[1], fracCrops_nonIrrLandDemand[2], fracCrops_nonIrrLandDemand[3], fracCrops_nonIrrLandDemand[4], fracCrops_nonIrrLandDemand[5], fracCrops_nonIrrLandDemand[6], fracCrops_nonIrrLandDemand[7], fracCrops_nonIrrLandDemand[8], fracCrops_nonIrrLandDemand[9], fracCrops_nonIrrLandDemand[10], fracCrops_nonIrrLandDemand[11], fracCrops_nonIrrLandDemand[12], fracCrops_nonIrrLandDemand[13], fracCrops_nonIrrLandDemand[14], fracCrops_nonIrrLandDemand[15], fracCrops_nonIrrLandDemand[16], fracCrops_nonIrrLandDemand[17], fallowIrr, fallownonIrr, GeneralCrop_Irr, GeneralCrop_nonIrr, head_development, areaPaddy_Irr_segment, areaCrops_Irr_segment[0], areaCrops_nonIrr_segment[0], areaCrops_Irr_segment[1], areaCrops_nonIrr_segment[1], areaCrops_Irr_segment[2], areaCrops_nonIrr_segment[2], areaCrops_Irr_segment[3], areaCrops_nonIrr_segment[3], areaCrops_Irr_segment[4], areaCrops_nonIrr_segment[4], areaCrops_Irr_segment[5], areaCrops_nonIrr_segment[5], areaCrops_Irr_segment[6], areaCrops_nonIrr_segment[6], areaCrops_Irr_segment[7], areaCrops_nonIrr_segment[7], areaCrops_Irr_segment[8], areaCrops_nonIrr_segment[8], areaCrops_Irr_segment[9], areaCrops_nonIrr_segment[9], areaCrops_Irr_segment[10], areaCrops_nonIrr_segment[10], areaCrops_Irr_segment[11], areaCrops_nonIrr_segment[11], areaCrops_Irr_segment[12], areaCrops_nonIrr_segment[12], areaCrops_Irr_segment[13], areaCrops_nonIrr_segment[13], areaCrops_Irr_segment[14], areaCrops_nonIrr_segment[14], areaCrops_Irr_segment[15], areaCrops_nonIrr_segment[15] , areaCrops_Irr_segment[16], areaCrops_nonIrr_segment[16],  areaCrops_Irr_segment[17], areaCrops_nonIrr_segment[17], availableArableLand, availableArableLand_segment</t>
   </si>
   <si>
-    <t>waterBodyID, resVolume_reservoir, cellArea, adminSegments, GeneralCrop_Irr, modflowtotalSoilThickness</t>
-  </si>
-  <si>
-    <t>$(PathGroundwaterModflowOutput)/Bhima_steady_12Oct.hds</t>
-  </si>
-  <si>
-    <t>$(FILE_PATHS:PathMaps)/init/Bhima_20160501.nc</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 05/05/2015</t>
-  </si>
-  <si>
-    <t>$(FILE_PATHS:PathMaps)/init/Bhima_20150505.nc</t>
-  </si>
-  <si>
-    <t>act_irrWithdrawalSW, act_irrWithdrawalGW, act_nonIrrWithdrawalSW, act_nonIrrWithdrawalGW, actual_totalWithdrawal, actTransTotal_grasslands, actTransTotal_nonpaddy, discharge, act_irrWithdrawal, act_nonIrrWithdrawal</t>
-  </si>
-  <si>
-    <t>automaticFallowingIrr</t>
-  </si>
-  <si>
-    <t>True for MS, False for FUSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 30/05/2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 01/07/2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 30/04/2015</t>
+    <t xml:space="preserve"> 30/05/2010</t>
+  </si>
+  <si>
+    <t>$(PathGroundwaterModflowOutput)/Bhima_steady_17Oct.hds</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 02/01/1998</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 02/01/1995</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12/01/2007</t>
   </si>
 </sst>
 </file>
@@ -1723,11 +1699,11 @@
   <sheetPr>
     <tabColor rgb="FF636EFA"/>
   </sheetPr>
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1762,7 +1738,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="C2" s="48" t="s">
         <v>150</v>
@@ -1776,7 +1752,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="C3" s="48" t="s">
         <v>152</v>
@@ -1790,7 +1766,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="C4" s="48" t="s">
         <v>151</v>
@@ -1805,13 +1781,13 @@
         <v>18</v>
       </c>
       <c r="B5" s="51">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C5" s="48" t="s">
         <v>106</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1819,7 +1795,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="53">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C6" s="48" t="s">
         <v>101</v>
@@ -1845,7 +1821,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="53" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C8" s="48" t="s">
         <v>156</v>
@@ -1901,7 +1877,7 @@
         <v>27</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="C12" s="48" t="s">
         <v>159</v>
@@ -1915,7 +1891,7 @@
         <v>28</v>
       </c>
       <c r="B13" s="54" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C13" s="48" t="s">
         <v>162</v>
@@ -2033,7 +2009,7 @@
         <v>12</v>
       </c>
       <c r="B21" s="60" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="C21" s="57" t="s">
         <v>137</v>
@@ -2042,7 +2018,7 @@
         <v>138</v>
       </c>
       <c r="E21" s="60" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="F21" s="60" t="s">
         <v>205</v>
@@ -2056,7 +2032,7 @@
         <v>13</v>
       </c>
       <c r="B22" s="47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="57" t="s">
         <v>99</v>
@@ -2084,7 +2060,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="47" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C24" s="57" t="s">
         <v>108</v>
@@ -2098,7 +2074,7 @@
         <v>47</v>
       </c>
       <c r="B25" s="61" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C25" s="57" t="s">
         <v>136</v>
@@ -2210,7 +2186,7 @@
         <v>196</v>
       </c>
       <c r="K33" s="50" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2218,7 +2194,7 @@
         <v>198</v>
       </c>
       <c r="B34" s="53">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2250,66 +2226,32 @@
         <v>202</v>
       </c>
       <c r="B38" s="53">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="50" t="s">
-        <v>218</v>
-      </c>
-      <c r="B39" s="53" t="s">
-        <v>209</v>
+        <v>213</v>
+      </c>
+      <c r="B39" s="53" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="50" t="s">
+        <v>218</v>
+      </c>
+      <c r="B40" s="53" t="b">
+        <v>1</v>
+      </c>
+      <c r="C40" s="48" t="s">
         <v>219</v>
       </c>
-      <c r="B40" s="53" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="50" t="s">
+      <c r="D40" s="50" t="s">
+        <v>221</v>
+      </c>
+      <c r="E40" s="53" t="s">
         <v>222</v>
-      </c>
-      <c r="B41" s="53" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="50" t="s">
-        <v>220</v>
-      </c>
-      <c r="B42" s="53" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="50" t="s">
-        <v>221</v>
-      </c>
-      <c r="B43" s="53" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="50" t="s">
-        <v>223</v>
-      </c>
-      <c r="B44" s="53" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="50" t="s">
-        <v>232</v>
-      </c>
-      <c r="B45" s="53" t="b">
-        <v>1</v>
-      </c>
-      <c r="C45" s="48" t="s">
-        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -3218,7 +3160,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D18" s="23">
         <v>6</v>
@@ -3260,7 +3202,7 @@
         <v>0.2</v>
       </c>
       <c r="R18" s="11" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.5">
@@ -3269,7 +3211,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D19" s="23">
         <v>11</v>

</xml_diff>